<commit_message>
Hago este commit para guardar algunos cambios, me está dando problemas de visibilidad de elementos esta rama.
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC73EFA2-66DB-410B-9701-02FA59D7E09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE123325-0FBA-4FFF-971C-9707EF2C83A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-4020" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="2246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="2247">
   <si>
     <t>Hogar</t>
   </si>
@@ -6777,6 +6777,9 @@
   </si>
   <si>
     <t>SAI</t>
+  </si>
+  <si>
+    <t>En el hogar</t>
   </si>
 </sst>
 </file>
@@ -7176,7 +7179,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D1" sqref="D1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7221,10 +7224,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>304</v>
+        <v>260</v>
       </c>
       <c r="C2" s="3">
-        <v>45027</v>
+        <v>45051</v>
       </c>
       <c r="D2" t="s">
         <v>2244</v>
@@ -7234,11 +7237,11 @@
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F8" si="0">CONCATENATE(TEXT(B2,"0000"),"/",TEXT(H2,"00"))</f>
-        <v>0304/01</v>
+        <v>0260/01</v>
       </c>
       <c r="G2" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F2),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>776a5681-3036-49e1-84db-df88b3d52a1d</v>
+        <v>1e98d195-38fa-4cee-9e2b-8731c2d972a9</v>
       </c>
       <c r="H2" s="5">
         <v>1</v>
@@ -7249,10 +7252,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>269</v>
+        <v>202</v>
       </c>
       <c r="C3" s="3">
-        <v>45030</v>
+        <v>45055</v>
       </c>
       <c r="D3" t="s">
         <v>2244</v>
@@ -7262,11 +7265,11 @@
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
-        <v>0269/01</v>
+        <v>0202/01</v>
       </c>
       <c r="G3" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F3),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>3a7f1148-3157-4426-8a96-f391a973cfdc</v>
+        <v>a1f9cfc2-51c2-417b-8177-42ccc628d275</v>
       </c>
       <c r="H3" s="5">
         <v>1</v>
@@ -7277,10 +7280,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C4" s="3">
-        <v>45020</v>
+        <v>45048</v>
       </c>
       <c r="D4" t="s">
         <v>2244</v>
@@ -7290,14 +7293,14 @@
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>0094/05</v>
+        <v>0074/01</v>
       </c>
       <c r="G4" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F4),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>ba1c2c33-ed90-429f-b3a1-d96147dfcf11</v>
+        <v>a1e86953-4223-48c3-86df-3c3f419e4d02</v>
       </c>
       <c r="H4" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -7305,10 +7308,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>70</v>
+        <v>264</v>
       </c>
       <c r="C5" s="3">
-        <v>45027</v>
+        <v>45054</v>
       </c>
       <c r="D5" t="s">
         <v>2244</v>
@@ -7318,14 +7321,14 @@
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>0070/02</v>
+        <v>0264/01</v>
       </c>
       <c r="G5" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F5),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>e069d11c-5e65-4ba3-ba65-8bc1adce2860</v>
+        <v>54df74b3-ece6-4abd-ad99-264478ff1323</v>
       </c>
       <c r="H5" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -7333,24 +7336,24 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>173</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3">
-        <v>45029</v>
+        <v>45055</v>
       </c>
       <c r="D6" t="s">
         <v>2244</v>
       </c>
       <c r="E6" t="s">
-        <v>2245</v>
+        <v>2246</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>0173/01</v>
+        <v>0016/01</v>
       </c>
       <c r="G6" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F6),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>2e445697-e499-490b-ba40-6ab9412e82d0</v>
+        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
       </c>
       <c r="H6" s="5">
         <v>1</v>
@@ -7361,10 +7364,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>288</v>
+        <v>148</v>
       </c>
       <c r="C7" s="3">
-        <v>45027</v>
+        <v>45054</v>
       </c>
       <c r="D7" t="s">
         <v>2244</v>
@@ -7374,11 +7377,11 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>0288/01</v>
+        <v>0148/01</v>
       </c>
       <c r="G7" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F7),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>8d61f76a-54b3-49fb-8bf4-760705670b34</v>
+        <v>544b8ff7-f2df-4584-8c9d-fe746daea693</v>
       </c>
       <c r="H7" s="5">
         <v>1</v>
@@ -7389,10 +7392,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>266</v>
+        <v>106</v>
       </c>
       <c r="C8" s="3">
-        <v>45027</v>
+        <v>45050</v>
       </c>
       <c r="D8" t="s">
         <v>2244</v>
@@ -7402,14 +7405,14 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>0266/01</v>
+        <v>0106/02</v>
       </c>
       <c r="G8" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F8),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>11116350-a3f7-4ed1-9f4b-503a433d5262</v>
+        <v>77c51c15-e6a1-4fef-b5bd-9bb349469be4</v>
       </c>
       <c r="H8" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -7417,24 +7420,24 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="C9" s="3">
-        <v>45020</v>
+        <v>45050</v>
       </c>
       <c r="D9" t="s">
         <v>2244</v>
       </c>
       <c r="E9" t="s">
-        <v>2245</v>
+        <v>2246</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" ref="F9:F13" si="1">CONCATENATE(TEXT(B9,"0000"),"/",TEXT(H9,"00"))</f>
-        <v>0024/01</v>
+        <v>0141/01</v>
       </c>
       <c r="G9" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F9),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>1e7ab3f1-c9bb-4930-8649-1e5b29241974</v>
+        <v>4cee805b-83d5-42e4-8b05-0ed3585fd1ce</v>
       </c>
       <c r="H9" s="5">
         <v>1</v>
@@ -7445,27 +7448,27 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>33</v>
+        <v>176</v>
       </c>
       <c r="C10" s="3">
-        <v>45035</v>
+        <v>45048</v>
       </c>
       <c r="D10" t="s">
         <v>2244</v>
       </c>
       <c r="E10" t="s">
-        <v>2245</v>
+        <v>2246</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
-        <v>0033/01</v>
+        <v>0176/02</v>
       </c>
       <c r="G10" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F10),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>a573c7cc-3952-4261-8a03-4b5ecb553281</v>
+        <v>8bf15d31-813f-40cc-824b-5ea8e3a93ee7</v>
       </c>
       <c r="H10" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -7473,10 +7476,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>86</v>
+        <v>201</v>
       </c>
       <c r="C11" s="3">
-        <v>45020</v>
+        <v>45056</v>
       </c>
       <c r="D11" t="s">
         <v>2244</v>
@@ -7486,11 +7489,11 @@
       </c>
       <c r="F11" t="str">
         <f t="shared" ref="F11" si="2">CONCATENATE(TEXT(B11,"0000"),"/",TEXT(H11,"00"))</f>
-        <v>0086/01</v>
+        <v>0201/01</v>
       </c>
       <c r="G11" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F11),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>74d14da7-190a-4785-b3ec-6a521b23b645</v>
+        <v>31c3a463-43ee-4c73-a048-41a6ad28c9aa</v>
       </c>
       <c r="H11" s="5">
         <v>1</v>
@@ -7501,10 +7504,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>15</v>
+        <v>307</v>
       </c>
       <c r="C12" s="3">
-        <v>45035</v>
+        <v>45049</v>
       </c>
       <c r="D12" t="s">
         <v>2244</v>
@@ -7514,11 +7517,11 @@
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
-        <v>0015/01</v>
+        <v>0307/01</v>
       </c>
       <c r="G12" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F12),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>ecd10b34-acd7-4b78-8c9c-143437bbe248</v>
+        <v>cf49e82b-6698-4c1d-ac40-5afe2f20bc8d</v>
       </c>
       <c r="H12" s="5">
         <v>1</v>
@@ -7529,10 +7532,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>257</v>
+        <v>186</v>
       </c>
       <c r="C13" s="3">
-        <v>45034</v>
+        <v>45055</v>
       </c>
       <c r="D13" t="s">
         <v>2244</v>
@@ -7542,11 +7545,11 @@
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
-        <v>0257/01</v>
+        <v>0186/01</v>
       </c>
       <c r="G13" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F13),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>f42941d7-e985-4f40-a421-2b382ea69f20</v>
+        <v>f2bc44f2-a087-48e9-843c-12a43825ae0f</v>
       </c>
       <c r="H13" s="5">
         <v>1</v>
@@ -7557,10 +7560,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C14" s="3">
-        <v>45030</v>
+        <v>45055</v>
       </c>
       <c r="D14" t="s">
         <v>2244</v>
@@ -7570,14 +7573,14 @@
       </c>
       <c r="F14" t="str">
         <f>CONCATENATE(TEXT(B14,"0000"),"/",TEXT(H14,"00"))</f>
-        <v>0198/02</v>
+        <v>0192/01</v>
       </c>
       <c r="G14" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F14),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>dece9b58-ae3b-404e-bbab-745c08d6be4e</v>
+        <v>755f34f5-c8d7-4162-bbfa-10a6e7a5a7df</v>
       </c>
       <c r="H14" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -7585,10 +7588,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>175</v>
+        <v>236</v>
       </c>
       <c r="C15" s="3">
-        <v>45033</v>
+        <v>45056</v>
       </c>
       <c r="D15" t="s">
         <v>2244</v>
@@ -7598,14 +7601,14 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" ref="F15" si="3">CONCATENATE(TEXT(B15,"0000"),"/",TEXT(H15,"00"))</f>
-        <v>0175/02</v>
+        <v>0236/01</v>
       </c>
       <c r="G15" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F15),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>c2dbbaf4-a305-4cc0-9a02-2611482b3406</v>
+        <v>996bb6cf-3cf9-46ac-8e8e-61a23ac5747e</v>
       </c>
       <c r="H15" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ya empecé las pruebas desde los archivos funciones y elementos a un archivo notebook, luego debo empezar en un archivo .py para ir dejando de usar el archivo digitar_06
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE123325-0FBA-4FFF-971C-9707EF2C83A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C7B4AC-2943-4E4C-BA53-0F1EA7DB3779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="2247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="2251">
   <si>
     <t>Hogar</t>
   </si>
@@ -6776,10 +6776,22 @@
     <t>Seguimiento</t>
   </si>
   <si>
-    <t>SAI</t>
-  </si>
-  <si>
     <t>En el hogar</t>
+  </si>
+  <si>
+    <t>Motivo de la visita:</t>
+  </si>
+  <si>
+    <t>Visita regular</t>
+  </si>
+  <si>
+    <t>Monitoreo posterior a la graduación</t>
+  </si>
+  <si>
+    <t>Donde se entrgaron:</t>
+  </si>
+  <si>
+    <t>En el SAI</t>
   </si>
 </sst>
 </file>
@@ -6833,13 +6845,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7176,10 +7191,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:J1048576"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7224,24 +7239,24 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>260</v>
+        <v>111</v>
       </c>
       <c r="C2" s="3">
-        <v>45051</v>
+        <v>45057</v>
       </c>
       <c r="D2" t="s">
         <v>2244</v>
       </c>
       <c r="E2" t="s">
-        <v>2245</v>
+        <v>2250</v>
       </c>
       <c r="F2" t="str">
-        <f t="shared" ref="F2:F8" si="0">CONCATENATE(TEXT(B2,"0000"),"/",TEXT(H2,"00"))</f>
-        <v>0260/01</v>
+        <f t="shared" ref="F2:F4" si="0">CONCATENATE(TEXT(B2,"0000"),"/",TEXT(H2,"00"))</f>
+        <v>0111/01</v>
       </c>
       <c r="G2" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F2),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>1e98d195-38fa-4cee-9e2b-8731c2d972a9</v>
+        <v>c6674d90-1e86-405b-b19c-5a8c0bce0841</v>
       </c>
       <c r="H2" s="5">
         <v>1</v>
@@ -7252,24 +7267,24 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="C3" s="3">
-        <v>45055</v>
+        <v>45057</v>
       </c>
       <c r="D3" t="s">
         <v>2244</v>
       </c>
       <c r="E3" t="s">
-        <v>2245</v>
+        <v>2250</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
-        <v>0202/01</v>
+        <v>0166/01</v>
       </c>
       <c r="G3" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F3),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>a1f9cfc2-51c2-417b-8177-42ccc628d275</v>
+        <v>57221e96-7586-449e-b6b4-58528e9cfc19</v>
       </c>
       <c r="H3" s="5">
         <v>1</v>
@@ -7280,334 +7295,26 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>74</v>
+        <v>217</v>
       </c>
       <c r="C4" s="3">
-        <v>45048</v>
+        <v>45057</v>
       </c>
       <c r="D4" t="s">
         <v>2244</v>
       </c>
       <c r="E4" t="s">
-        <v>2245</v>
+        <v>2250</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>0074/01</v>
+        <v>0217/01</v>
       </c>
       <c r="G4" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F4),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>a1e86953-4223-48c3-86df-3c3f419e4d02</v>
+        <v>910cf6fd-692e-4ac4-abcb-674bfcbe4122</v>
       </c>
       <c r="H4" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>264</v>
-      </c>
-      <c r="C5" s="3">
-        <v>45054</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>0264/01</v>
-      </c>
-      <c r="G5" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F5),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>54df74b3-ece6-4abd-ad99-264478ff1323</v>
-      </c>
-      <c r="H5" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3">
-        <v>45055</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2246</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>0016/01</v>
-      </c>
-      <c r="G6" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F6),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
-      </c>
-      <c r="H6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>148</v>
-      </c>
-      <c r="C7" s="3">
-        <v>45054</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>0148/01</v>
-      </c>
-      <c r="G7" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F7),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>544b8ff7-f2df-4584-8c9d-fe746daea693</v>
-      </c>
-      <c r="H7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>106</v>
-      </c>
-      <c r="C8" s="3">
-        <v>45050</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>0106/02</v>
-      </c>
-      <c r="G8" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F8),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>77c51c15-e6a1-4fef-b5bd-9bb349469be4</v>
-      </c>
-      <c r="H8" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>141</v>
-      </c>
-      <c r="C9" s="3">
-        <v>45050</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2246</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" ref="F9:F13" si="1">CONCATENATE(TEXT(B9,"0000"),"/",TEXT(H9,"00"))</f>
-        <v>0141/01</v>
-      </c>
-      <c r="G9" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F9),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>4cee805b-83d5-42e4-8b05-0ed3585fd1ce</v>
-      </c>
-      <c r="H9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1">
-        <v>176</v>
-      </c>
-      <c r="C10" s="3">
-        <v>45048</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2246</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="1"/>
-        <v>0176/02</v>
-      </c>
-      <c r="G10" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F10),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>8bf15d31-813f-40cc-824b-5ea8e3a93ee7</v>
-      </c>
-      <c r="H10" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1">
-        <v>201</v>
-      </c>
-      <c r="C11" s="3">
-        <v>45056</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" ref="F11" si="2">CONCATENATE(TEXT(B11,"0000"),"/",TEXT(H11,"00"))</f>
-        <v>0201/01</v>
-      </c>
-      <c r="G11" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F11),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>31c3a463-43ee-4c73-a048-41a6ad28c9aa</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
-        <v>307</v>
-      </c>
-      <c r="C12" s="3">
-        <v>45049</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="1"/>
-        <v>0307/01</v>
-      </c>
-      <c r="G12" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F12),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>cf49e82b-6698-4c1d-ac40-5afe2f20bc8d</v>
-      </c>
-      <c r="H12" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1">
-        <v>186</v>
-      </c>
-      <c r="C13" s="3">
-        <v>45055</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="1"/>
-        <v>0186/01</v>
-      </c>
-      <c r="G13" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F13),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>f2bc44f2-a087-48e9-843c-12a43825ae0f</v>
-      </c>
-      <c r="H13" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1">
-        <v>192</v>
-      </c>
-      <c r="C14" s="3">
-        <v>45055</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E14" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F14" t="str">
-        <f>CONCATENATE(TEXT(B14,"0000"),"/",TEXT(H14,"00"))</f>
-        <v>0192/01</v>
-      </c>
-      <c r="G14" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F14),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>755f34f5-c8d7-4162-bbfa-10a6e7a5a7df</v>
-      </c>
-      <c r="H14" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1">
-        <v>236</v>
-      </c>
-      <c r="C15" s="3">
-        <v>45056</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E15" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" ref="F15" si="3">CONCATENATE(TEXT(B15,"0000"),"/",TEXT(H15,"00"))</f>
-        <v>0236/01</v>
-      </c>
-      <c r="G15" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F15),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>996bb6cf-3cf9-46ac-8e8e-61a23ac5747e</v>
-      </c>
-      <c r="H15" s="5">
         <v>1</v>
       </c>
     </row>
@@ -7625,19 +7332,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF1EAA0-8A30-4F1C-A86F-F04BCE344154}">
-  <dimension ref="A1:B1118"/>
+  <dimension ref="A1:E1118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2242</v>
       </c>
@@ -7645,31 +7354,43 @@
         <v>2241</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>596</v>
       </c>
       <c r="B2" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" s="6" t="s">
+        <v>2246</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2228</v>
       </c>
       <c r="B3" t="s">
         <v>2227</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>2244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2000</v>
       </c>
       <c r="B4" t="s">
         <v>1999</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>2248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1894</v>
       </c>
@@ -7677,23 +7398,32 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1612</v>
       </c>
       <c r="B6" t="s">
         <v>1611</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6" s="6" t="s">
+        <v>2249</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1342</v>
       </c>
       <c r="B7" t="s">
         <v>1341</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1840</v>
       </c>
@@ -7701,7 +7431,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>558</v>
       </c>
@@ -7709,7 +7439,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2008</v>
       </c>
@@ -7717,7 +7447,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1184</v>
       </c>
@@ -7725,7 +7455,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1324</v>
       </c>
@@ -7733,7 +7463,7 @@
         <v>1323</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>470</v>
       </c>
@@ -7741,7 +7471,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -7749,7 +7479,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -7757,7 +7487,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>892</v>
       </c>

</xml_diff>

<commit_message>
Eliminé las funciones 'firma' y 'visita', las implementé directamente en la función encabezado. Segmenté el origen de información de los servicios para segmentarlos por columnas y convertirlos en listas, esos cambios se ven reflejados en las funciones que usan esta información.
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C7B4AC-2943-4E4C-BA53-0F1EA7DB3779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F342FB74-503B-496E-8CCB-D2CB05CE9E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="2251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2293" uniqueCount="2283">
   <si>
     <t>Hogar</t>
   </si>
@@ -6792,6 +6792,102 @@
   </si>
   <si>
     <t>En el SAI</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0308/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0308/02</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0308/03</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0308/04</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0309/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0309/02</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0309/03</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0309/04</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0310/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0310/02</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0310/03</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0310/04</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0311/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0311/02</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0311/03</t>
+  </si>
+  <si>
+    <t>64277d0e-97da-446d-a687-0d7ea0fe64b3</t>
+  </si>
+  <si>
+    <t>8875a779-0a18-4aed-86ba-1b03b378e439</t>
+  </si>
+  <si>
+    <t>e3a0cbf8-6de8-4627-9384-f02a496569d4</t>
+  </si>
+  <si>
+    <t>33133711-ae3f-4166-959b-4b99ab79d07d</t>
+  </si>
+  <si>
+    <t>c128fd59-88ae-4ebe-9569-15be7e13b096</t>
+  </si>
+  <si>
+    <t>7e1d7969-7da4-4889-b4f6-aaeae9d46961</t>
+  </si>
+  <si>
+    <t>19036049-ad12-456e-8fe0-9527f021ce80</t>
+  </si>
+  <si>
+    <t>fbc2cb3c-477a-4933-95ba-09d4c1d2c4cb</t>
+  </si>
+  <si>
+    <t>11e39041-f9fd-45b6-94b8-c301b9910979</t>
+  </si>
+  <si>
+    <t>1769f7e0-f29c-4795-83d6-7a8838da5757</t>
+  </si>
+  <si>
+    <t>b70bc750-687b-4d7a-80fc-2210aa945b09</t>
+  </si>
+  <si>
+    <t>e7e0bf58-c6b2-42dc-a78f-0e9b8ae98e47</t>
+  </si>
+  <si>
+    <t>fc8be43a-4d54-457b-a84b-406a829a0135</t>
+  </si>
+  <si>
+    <t>381e38e5-745b-4249-93de-de7da7aae679</t>
+  </si>
+  <si>
+    <t>e9d0910c-e2cf-4ba4-b694-b66edeaf45d3</t>
+  </si>
+  <si>
+    <t>En el Hogar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seguimiento </t>
   </si>
 </sst>
 </file>
@@ -7191,10 +7287,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7239,7 +7335,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>111</v>
+        <v>310</v>
       </c>
       <c r="C2" s="3">
         <v>45057</v>
@@ -7251,12 +7347,12 @@
         <v>2250</v>
       </c>
       <c r="F2" t="str">
-        <f t="shared" ref="F2:F4" si="0">CONCATENATE(TEXT(B2,"0000"),"/",TEXT(H2,"00"))</f>
-        <v>0111/01</v>
+        <f t="shared" ref="F2:F7" si="0">CONCATENATE(TEXT(B2,"0000"),"/",TEXT(H2,"00"))</f>
+        <v>0310/01</v>
       </c>
       <c r="G2" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F2),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>c6674d90-1e86-405b-b19c-5a8c0bce0841</v>
+        <v>11e39041-f9fd-45b6-94b8-c301b9910979</v>
       </c>
       <c r="H2" s="5">
         <v>1</v>
@@ -7267,24 +7363,24 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>166</v>
+        <v>311</v>
       </c>
       <c r="C3" s="3">
-        <v>45057</v>
+        <v>45061</v>
       </c>
       <c r="D3" t="s">
         <v>2244</v>
       </c>
       <c r="E3" t="s">
-        <v>2250</v>
+        <v>2281</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
-        <v>0166/01</v>
+        <v>0311/01</v>
       </c>
       <c r="G3" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F3),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>57221e96-7586-449e-b6b4-58528e9cfc19</v>
+        <v>fc8be43a-4d54-457b-a84b-406a829a0135</v>
       </c>
       <c r="H3" s="5">
         <v>1</v>
@@ -7295,7 +7391,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>217</v>
+        <v>116</v>
       </c>
       <c r="C4" s="3">
         <v>45057</v>
@@ -7308,13 +7404,97 @@
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>0217/01</v>
+        <v>0116/01</v>
       </c>
       <c r="G4" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F4),Sheet1!$A$1:$B$1250,2,FALSE)</f>
-        <v>910cf6fd-692e-4ac4-abcb-674bfcbe4122</v>
+        <v>e4f096e5-c705-45a1-8ac8-79761d421d5f</v>
       </c>
       <c r="H4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>290</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45058</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2250</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>0290/01</v>
+      </c>
+      <c r="G5" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F5),Sheet1!$A$1:$B$1250,2,FALSE)</f>
+        <v>3c0ffb38-6a59-444f-b374-cdd857571011</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>143</v>
+      </c>
+      <c r="C6" s="3">
+        <v>45061</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2250</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>0143/01</v>
+      </c>
+      <c r="G6" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F6),Sheet1!$A$1:$B$1250,2,FALSE)</f>
+        <v>7dd3328d-6a3d-4fe4-b2b1-efda4799a5ad</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>256</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45058</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2282</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2250</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>0256/01</v>
+      </c>
+      <c r="G7" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F7),Sheet1!$A$1:$B$1250,2,FALSE)</f>
+        <v>ea21c93d-c38a-47f1-b12e-f1f4337c11be</v>
+      </c>
+      <c r="H7" s="5">
         <v>1</v>
       </c>
     </row>
@@ -7332,10 +7512,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF1EAA0-8A30-4F1C-A86F-F04BCE344154}">
-  <dimension ref="A1:E1118"/>
+  <dimension ref="A1:E1133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A1124" workbookViewId="0">
+      <selection activeCell="B1136" sqref="B1136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16311,6 +16491,126 @@
         <v>1775</v>
       </c>
     </row>
+    <row r="1119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1119" t="s">
+        <v>2251</v>
+      </c>
+      <c r="B1119" t="s">
+        <v>2266</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1120" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B1120" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1121" t="s">
+        <v>2253</v>
+      </c>
+      <c r="B1121" t="s">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1122" t="s">
+        <v>2254</v>
+      </c>
+      <c r="B1122" t="s">
+        <v>2269</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1123" t="s">
+        <v>2255</v>
+      </c>
+      <c r="B1123" t="s">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1124" t="s">
+        <v>2256</v>
+      </c>
+      <c r="B1124" t="s">
+        <v>2271</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1125" t="s">
+        <v>2257</v>
+      </c>
+      <c r="B1125" t="s">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1126" t="s">
+        <v>2258</v>
+      </c>
+      <c r="B1126" t="s">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1127" t="s">
+        <v>2259</v>
+      </c>
+      <c r="B1127" t="s">
+        <v>2274</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1128" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B1128" t="s">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1129" t="s">
+        <v>2261</v>
+      </c>
+      <c r="B1129" t="s">
+        <v>2276</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1130" t="s">
+        <v>2262</v>
+      </c>
+      <c r="B1130" t="s">
+        <v>2277</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1131" t="s">
+        <v>2263</v>
+      </c>
+      <c r="B1131" t="s">
+        <v>2278</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1132" t="s">
+        <v>2264</v>
+      </c>
+      <c r="B1132" t="s">
+        <v>2279</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1133" t="s">
+        <v>2265</v>
+      </c>
+      <c r="B1133" t="s">
+        <v>2280</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B1118" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B1118">

</xml_diff>

<commit_message>
Se agregaron funciones para recorrer mas de un servicio y mejoras en el codigo con el uso de estructuras de datos
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F342FB74-503B-496E-8CCB-D2CB05CE9E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38517D3-91FC-4837-949B-AED0513FBBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
@@ -7290,7 +7290,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7299,8 +7299,8 @@
     <col min="3" max="3" width="11.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="38.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="38.28515625" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="5"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Corrección en la funcion 'Servir', se agregó un contador para ir viendo el avance de lo digitado
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeniel\Documents\Programación\Python\Shaka\data_entry_achieve\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2940448F-3E90-4A54-9B94-FA52C498EE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB145E91-F5DA-4FA7-AAB7-207FEC4D49CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -6887,27 +6887,15 @@
     <t>Serv1</t>
   </si>
   <si>
-    <t xml:space="preserve">Dnr1 </t>
-  </si>
-  <si>
     <t>Serv2</t>
   </si>
   <si>
-    <t>Dnr2</t>
-  </si>
-  <si>
     <t>Serv3</t>
   </si>
   <si>
-    <t>Dnr3</t>
-  </si>
-  <si>
     <t>Serv4</t>
   </si>
   <si>
-    <t>Dnr4</t>
-  </si>
-  <si>
     <t>1.40</t>
   </si>
   <si>
@@ -6924,6 +6912,18 @@
   </si>
   <si>
     <t>3bb419e9-3b73-4f1b-94b4-a80f7fd72afc</t>
+  </si>
+  <si>
+    <t>Don1</t>
+  </si>
+  <si>
+    <t>Don2</t>
+  </si>
+  <si>
+    <t>Don3</t>
+  </si>
+  <si>
+    <t>Don4</t>
   </si>
 </sst>
 </file>
@@ -7325,8 +7325,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7373,25 +7373,25 @@
         <v>2281</v>
       </c>
       <c r="J1" t="s">
+        <v>2291</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>2282</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" t="s">
+        <v>2292</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>2283</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
+        <v>2293</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>2284</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="N1" t="s">
-        <v>2286</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>2287</v>
-      </c>
       <c r="P1" t="s">
-        <v>2288</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -7422,28 +7422,28 @@
         <v>2</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L2">
         <v>9</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -7474,28 +7474,28 @@
         <v>5</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J3" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L3">
         <v>6</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N3">
         <v>9</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P3" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -7526,28 +7526,28 @@
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J4" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L4">
         <v>6</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N4">
         <v>9</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P4" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -7578,28 +7578,28 @@
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J5" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L5">
         <v>6</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N5">
         <v>9</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P5" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -7630,28 +7630,28 @@
         <v>4</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J6" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L6">
         <v>6</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N6">
         <v>9</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P6" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="Q6" s="2"/>
     </row>
@@ -7683,28 +7683,28 @@
         <v>3</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J7" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L7">
         <v>6</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N7">
         <v>9</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P7" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="Q7" s="2"/>
     </row>
@@ -7736,28 +7736,28 @@
         <v>2</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J8" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L8">
         <v>6</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N8">
         <v>9</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P8" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -7788,28 +7788,28 @@
         <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J9" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L9">
         <v>6</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N9">
         <v>9</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P9" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -7840,28 +7840,28 @@
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J10" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L10">
         <v>6</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N10">
         <v>9</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P10" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -7892,28 +7892,28 @@
         <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J11" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L11">
         <v>6</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N11">
         <v>9</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P11" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -7944,28 +7944,28 @@
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J12" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L12">
         <v>6</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N12">
         <v>9</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P12" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -7996,28 +7996,28 @@
         <v>2</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J13" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L13">
         <v>6</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N13">
         <v>9</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P13" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -8048,28 +8048,28 @@
         <v>2</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J14" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L14">
         <v>6</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N14">
         <v>9</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P14" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -8100,28 +8100,28 @@
         <v>2</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J15" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L15">
         <v>6</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N15">
         <v>9</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P15" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -8152,28 +8152,28 @@
         <v>1</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J16" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L16">
         <v>6</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N16">
         <v>9</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P16" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -8204,28 +8204,28 @@
         <v>1</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J17" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L17">
         <v>6</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N17">
         <v>9</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P17" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -8256,28 +8256,28 @@
         <v>2</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J18" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L18">
         <v>6</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N18">
         <v>9</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P18" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -8308,28 +8308,28 @@
         <v>1</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J19" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L19">
         <v>6</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N19">
         <v>9</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P19" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -8360,28 +8360,28 @@
         <v>1</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J20" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L20">
         <v>6</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N20">
         <v>9</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P20" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -8412,28 +8412,28 @@
         <v>1</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J21" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L21">
         <v>6</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N21">
         <v>9</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P21" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -8464,28 +8464,28 @@
         <v>1</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J22" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="L22">
         <v>6</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="N22">
         <v>9</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P22" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -8516,28 +8516,28 @@
         <v>6</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J23" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L23">
         <v>9</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N23" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P23" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="Q23" s="2"/>
     </row>
@@ -8569,28 +8569,28 @@
         <v>1</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J24" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L24">
         <v>9</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N24" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P24" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -8621,28 +8621,28 @@
         <v>1</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J25" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L25">
         <v>9</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N25" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P25" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -8673,28 +8673,28 @@
         <v>1</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J26" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L26">
         <v>9</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N26" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P26" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -8725,28 +8725,28 @@
         <v>1</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J27" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L27">
         <v>9</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N27" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P27" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -8777,28 +8777,28 @@
         <v>1</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J28" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L28">
         <v>9</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N28" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P28" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -8829,28 +8829,28 @@
         <v>2</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J29" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L29">
         <v>9</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N29" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P29" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -8881,28 +8881,28 @@
         <v>1</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J30" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L30">
         <v>9</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N30" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P30" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -8933,28 +8933,28 @@
         <v>1</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J31" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L31">
         <v>9</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N31" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P31" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -8985,28 +8985,28 @@
         <v>1</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J32" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L32">
         <v>9</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N32" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P32" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -9037,28 +9037,28 @@
         <v>1</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J33" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L33">
         <v>9</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N33" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P33" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -9089,28 +9089,28 @@
         <v>2</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J34" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L34">
         <v>9</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N34" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P34" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -9141,28 +9141,28 @@
         <v>2</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J35" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L35">
         <v>9</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N35" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P35" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -9193,28 +9193,28 @@
         <v>1</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J36" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L36">
         <v>9</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N36" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P36" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -9245,28 +9245,28 @@
         <v>1</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J37" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L37">
         <v>9</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N37" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P37" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -9297,28 +9297,28 @@
         <v>1</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J38" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L38">
         <v>9</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N38" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P38" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -9349,28 +9349,28 @@
         <v>1</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J39" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L39">
         <v>9</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N39" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P39" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -9401,28 +9401,28 @@
         <v>2</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J40" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L40">
         <v>9</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N40" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P40" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -9453,28 +9453,28 @@
         <v>1</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J41" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L41">
         <v>9</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N41" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P41" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -9505,28 +9505,28 @@
         <v>2</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J42" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L42">
         <v>9</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N42" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P42" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -9557,28 +9557,28 @@
         <v>1</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J43" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L43">
         <v>9</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N43" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P43" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -9609,28 +9609,28 @@
         <v>4</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J44" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L44">
         <v>9</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N44" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P44" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -9661,28 +9661,28 @@
         <v>1</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J45" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L45">
         <v>9</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N45" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P45" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -9713,28 +9713,28 @@
         <v>1</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J46" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L46">
         <v>9</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N46" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P46" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -9754,7 +9754,7 @@
         <v>2245</v>
       </c>
       <c r="F47" s="2" t="str">
-        <f t="shared" ref="F47:F99" si="2">CONCATENATE(TEXT(B47,"0000"),"/",TEXT(H47,"00"))</f>
+        <f t="shared" ref="F47:F86" si="2">CONCATENATE(TEXT(B47,"0000"),"/",TEXT(H47,"00"))</f>
         <v>0212/01</v>
       </c>
       <c r="G47" t="str">
@@ -9765,28 +9765,28 @@
         <v>1</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J47" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L47">
         <v>9</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N47" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P47" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -9817,28 +9817,28 @@
         <v>1</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J48" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L48">
         <v>9</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N48" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P48" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -9869,28 +9869,28 @@
         <v>1</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J49" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L49">
         <v>9</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N49" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P49" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -9921,28 +9921,28 @@
         <v>7</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J50" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L50">
         <v>9</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N50" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P50" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="Q50" s="2"/>
     </row>
@@ -9974,28 +9974,28 @@
         <v>1</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J51" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L51">
         <v>9</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N51" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P51" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -10026,28 +10026,28 @@
         <v>1</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J52" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L52">
         <v>9</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N52" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P52" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
@@ -10078,28 +10078,28 @@
         <v>1</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J53" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L53">
         <v>9</v>
       </c>
       <c r="M53" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N53" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P53" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
@@ -10130,28 +10130,28 @@
         <v>1</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J54" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L54">
         <v>9</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N54" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P54" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
@@ -10182,28 +10182,28 @@
         <v>1</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J55" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L55">
         <v>9</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N55" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P55" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
@@ -10234,28 +10234,28 @@
         <v>1</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J56" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L56">
         <v>9</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N56" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P56" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
@@ -10286,28 +10286,28 @@
         <v>2</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J57" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L57">
         <v>9</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N57" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O57" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P57" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -10338,28 +10338,28 @@
         <v>1</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J58" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L58">
         <v>9</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N58" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P58" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
@@ -10390,28 +10390,28 @@
         <v>1</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J59" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L59">
         <v>9</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N59" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P59" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
@@ -10442,28 +10442,28 @@
         <v>1</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J60" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L60">
         <v>9</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N60" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O60" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P60" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
@@ -10494,28 +10494,28 @@
         <v>5</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J61" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L61">
         <v>9</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N61" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O61" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P61" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
@@ -10546,28 +10546,28 @@
         <v>1</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J62" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L62">
         <v>9</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N62" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O62" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P62" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
@@ -10598,28 +10598,28 @@
         <v>1</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J63" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L63">
         <v>9</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N63" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P63" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -10650,28 +10650,28 @@
         <v>1</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J64" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L64">
         <v>9</v>
       </c>
       <c r="M64" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N64" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O64" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P64" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
@@ -10702,28 +10702,28 @@
         <v>1</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J65" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L65">
         <v>9</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N65" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O65" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P65" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
@@ -10754,28 +10754,28 @@
         <v>1</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J66" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L66">
         <v>9</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N66" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O66" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P66" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -10806,28 +10806,28 @@
         <v>1</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J67" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L67">
         <v>9</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N67" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O67" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P67" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
@@ -10858,28 +10858,28 @@
         <v>1</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J68" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L68">
         <v>9</v>
       </c>
       <c r="M68" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N68" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O68" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P68" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
@@ -10910,28 +10910,28 @@
         <v>1</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J69" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L69">
         <v>9</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N69" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O69" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P69" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
@@ -10962,28 +10962,28 @@
         <v>1</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J70" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L70">
         <v>9</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N70" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P70" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
@@ -11014,28 +11014,28 @@
         <v>1</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J71" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L71">
         <v>9</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N71" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O71" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P71" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
@@ -11066,28 +11066,28 @@
         <v>1</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J72" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L72">
         <v>9</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N72" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O72" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P72" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -11118,28 +11118,28 @@
         <v>2</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J73" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L73">
         <v>9</v>
       </c>
       <c r="M73" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N73" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O73" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P73" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -11170,28 +11170,28 @@
         <v>1</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J74" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L74">
         <v>9</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N74" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O74" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P74" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -11222,28 +11222,28 @@
         <v>1</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J75" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L75">
         <v>9</v>
       </c>
       <c r="M75" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N75" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O75" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P75" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -11274,28 +11274,28 @@
         <v>1</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J76" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L76">
         <v>9</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N76" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P76" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -11326,28 +11326,28 @@
         <v>1</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J77" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K77" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L77">
         <v>9</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N77" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O77" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P77" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -11378,28 +11378,28 @@
         <v>1</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J78" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L78">
         <v>9</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N78" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O78" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P78" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
@@ -11430,28 +11430,28 @@
         <v>1</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J79" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L79">
         <v>9</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N79" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O79" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P79" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -11482,28 +11482,28 @@
         <v>1</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J80" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L80">
         <v>9</v>
       </c>
       <c r="M80" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N80" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O80" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P80" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
@@ -11534,28 +11534,28 @@
         <v>1</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J81" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L81">
         <v>9</v>
       </c>
       <c r="M81" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N81" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O81" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P81" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
@@ -11586,28 +11586,28 @@
         <v>1</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J82" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L82">
         <v>9</v>
       </c>
       <c r="M82" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N82" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O82" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P82" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
@@ -11638,28 +11638,28 @@
         <v>1</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>2292</v>
+        <v>2288</v>
       </c>
       <c r="J83" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L83">
         <v>9</v>
       </c>
       <c r="M83" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N83" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O83" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P83" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
@@ -11690,28 +11690,28 @@
         <v>2</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="J84">
         <v>6</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L84">
         <v>9</v>
       </c>
       <c r="M84" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N84" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P84" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
@@ -11742,28 +11742,28 @@
         <v>1</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="J85">
         <v>6</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L85">
         <v>9</v>
       </c>
       <c r="M85" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N85" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O85" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P85" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
@@ -11794,28 +11794,28 @@
         <v>1</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>2289</v>
+        <v>2285</v>
       </c>
       <c r="J86">
         <v>6</v>
       </c>
       <c r="K86" s="2" t="s">
-        <v>2290</v>
+        <v>2286</v>
       </c>
       <c r="L86">
         <v>9</v>
       </c>
       <c r="M86" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="N86" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="O86" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="P86" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
     </row>
   </sheetData>
@@ -18801,10 +18801,10 @@
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
-        <v>2293</v>
+        <v>2289</v>
       </c>
       <c r="B867" t="s">
-        <v>2294</v>
+        <v>2290</v>
       </c>
     </row>
     <row r="868" spans="1:2" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Preparado para el merge
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeniel\Documents\Programación\Python\Shaka\data_entry_achieve\Archivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB145E91-F5DA-4FA7-AAB7-207FEC4D49CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ACF921-BBAE-418A-BDFE-2FAD6F4EE0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$P$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$P$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$B$1134</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3033" uniqueCount="2295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2316" uniqueCount="2295">
   <si>
     <t>Hogar</t>
   </si>
@@ -7323,10 +7323,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:Q86"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7344,7 +7344,7 @@
     <col min="15" max="15" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -7394,7 +7394,7 @@
         <v>2294</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -7411,7 +7411,7 @@
         <v>2245</v>
       </c>
       <c r="F2" t="str">
-        <f t="shared" ref="F2:F33" si="0">CONCATENATE(TEXT(B2,"0000"),"/",TEXT(H2,"00"))</f>
+        <f t="shared" ref="F2:F4" si="0">CONCATENATE(TEXT(B2,"0000"),"/",TEXT(H2,"00"))</f>
         <v>0010/02</v>
       </c>
       <c r="G2" t="str">
@@ -7446,12 +7446,12 @@
         <v>2287</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C3" s="3">
         <v>45071</v>
@@ -7464,14 +7464,14 @@
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
-        <v>0049/05</v>
+        <v>0061/01</v>
       </c>
       <c r="G3" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F3),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>f1774a4b-b951-4693-8757-467334b011d9</v>
+        <v>b5ac990a-78e4-433d-9acd-c4acb6210d10</v>
       </c>
       <c r="H3" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>2288</v>
@@ -7498,12 +7498,12 @@
         <v>2287</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>61</v>
+        <v>228</v>
       </c>
       <c r="C4" s="3">
         <v>45071</v>
@@ -7516,11 +7516,11 @@
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>0061/01</v>
+        <v>0228/01</v>
       </c>
       <c r="G4" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F4),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>b5ac990a-78e4-433d-9acd-c4acb6210d10</v>
+        <v>bbfd3757-166f-4a75-a998-9c0ca6b58ef4</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -7550,4276 +7550,8 @@
         <v>2287</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>228</v>
-      </c>
-      <c r="C5" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>0228/01</v>
-      </c>
-      <c r="G5" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F5),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>bbfd3757-166f-4a75-a998-9c0ca6b58ef4</v>
-      </c>
-      <c r="H5" s="5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J5" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L5">
-        <v>6</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N5">
-        <v>9</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P5" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>247</v>
-      </c>
-      <c r="C6" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>0247/04</v>
-      </c>
-      <c r="G6" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F6),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>3bb419e9-3b73-4f1b-94b4-a80f7fd72afc</v>
-      </c>
-      <c r="H6" s="5">
-        <v>4</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J6" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L6">
-        <v>6</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N6">
-        <v>9</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P6" t="s">
-        <v>2287</v>
-      </c>
-      <c r="Q6" s="2"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>248</v>
-      </c>
-      <c r="C7" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>0248/03</v>
-      </c>
-      <c r="G7" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F7),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>f34a6d11-b3db-4744-987f-a7fe8961572b</v>
-      </c>
-      <c r="H7" s="5">
-        <v>3</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J7" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L7">
-        <v>6</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N7">
-        <v>9</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P7" t="s">
-        <v>2287</v>
-      </c>
-      <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>265</v>
-      </c>
-      <c r="C8" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0265/02</v>
-      </c>
-      <c r="G8" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F8),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>2bd6129c-7a32-4378-bdc1-0081eebbb548</v>
-      </c>
-      <c r="H8" s="5">
-        <v>2</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J8" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L8">
-        <v>6</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N8">
-        <v>9</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P8" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>287</v>
-      </c>
-      <c r="C9" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0287/01</v>
-      </c>
-      <c r="G9" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F9),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>e77ec9c4-ca74-4cca-8838-4c3b72c8d7e9</v>
-      </c>
-      <c r="H9" s="5">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J9" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L9">
-        <v>6</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N9">
-        <v>9</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P9" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1">
-        <v>292</v>
-      </c>
-      <c r="C10" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0292/01</v>
-      </c>
-      <c r="G10" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F10),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>81cd7611-ea1c-4580-964b-49b9fbb5d008</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J10" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L10">
-        <v>6</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N10">
-        <v>9</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P10" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1">
-        <v>296</v>
-      </c>
-      <c r="C11" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0296/01</v>
-      </c>
-      <c r="G11" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F11),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>519bb9e8-7948-451a-a8dd-2b92d420ae7f</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J11" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L11">
-        <v>6</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N11">
-        <v>9</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P11" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
-        <v>77</v>
-      </c>
-      <c r="C12" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0077/01</v>
-      </c>
-      <c r="G12" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F12),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>ad343fc9-75d0-4318-b21a-1d758a69dedc</v>
-      </c>
-      <c r="H12" s="5">
-        <v>1</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J12" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L12">
-        <v>6</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N12">
-        <v>9</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P12" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1">
-        <v>90</v>
-      </c>
-      <c r="C13" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0090/02</v>
-      </c>
-      <c r="G13" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F13),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>f389fdf6-5f88-437a-a4a4-0ae1f5c736f5</v>
-      </c>
-      <c r="H13" s="5">
-        <v>2</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J13" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L13">
-        <v>6</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N13">
-        <v>9</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P13" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1">
-        <v>96</v>
-      </c>
-      <c r="C14" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E14" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0096/02</v>
-      </c>
-      <c r="G14" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F14),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>f7946146-f3b4-472b-815e-4f90bd82b61b</v>
-      </c>
-      <c r="H14" s="5">
-        <v>2</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J14" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L14">
-        <v>6</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N14">
-        <v>9</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P14" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1">
-        <v>138</v>
-      </c>
-      <c r="C15" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E15" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0138/02</v>
-      </c>
-      <c r="G15" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F15),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>256dddaa-cfa8-4fa9-8493-8dde554450f9</v>
-      </c>
-      <c r="H15" s="5">
-        <v>2</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J15" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L15">
-        <v>6</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N15">
-        <v>9</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P15" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1">
-        <v>189</v>
-      </c>
-      <c r="C16" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D16" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0189/01</v>
-      </c>
-      <c r="G16" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F16),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>a78df1ea-8a08-44ab-9eba-610d12d56795</v>
-      </c>
-      <c r="H16" s="5">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J16" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L16">
-        <v>6</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N16">
-        <v>9</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P16" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1">
-        <v>191</v>
-      </c>
-      <c r="C17" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E17" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0191/01</v>
-      </c>
-      <c r="G17" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F17),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>ee3a9d9f-594f-4f62-ae4b-d22c7971a71a</v>
-      </c>
-      <c r="H17" s="5">
-        <v>1</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J17" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L17">
-        <v>6</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N17">
-        <v>9</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P17" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1">
-        <v>216</v>
-      </c>
-      <c r="C18" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E18" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0216/02</v>
-      </c>
-      <c r="G18" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F18),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>8877a927-e6b7-4f30-8779-e9da0888c551</v>
-      </c>
-      <c r="H18" s="5">
-        <v>2</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J18" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L18">
-        <v>6</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N18">
-        <v>9</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P18" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1">
-        <v>255</v>
-      </c>
-      <c r="C19" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D19" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E19" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0255/01</v>
-      </c>
-      <c r="G19" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F19),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>f464d37a-debc-4cc9-9dae-4b2ea2f8124a</v>
-      </c>
-      <c r="H19" s="5">
-        <v>1</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J19" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L19">
-        <v>6</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N19">
-        <v>9</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P19" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1">
-        <v>263</v>
-      </c>
-      <c r="C20" s="3">
-        <v>45073</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E20" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0263/01</v>
-      </c>
-      <c r="G20" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F20),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>3a711287-08cc-42e5-9699-ce108b4b7d25</v>
-      </c>
-      <c r="H20" s="5">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J20" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L20">
-        <v>6</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N20">
-        <v>9</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P20" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1">
-        <v>282</v>
-      </c>
-      <c r="C21" s="3">
-        <v>45073</v>
-      </c>
-      <c r="D21" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E21" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0282/01</v>
-      </c>
-      <c r="G21" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F21),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>917243cf-feab-4cbc-a0cb-73b302876708</v>
-      </c>
-      <c r="H21" s="5">
-        <v>1</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J21" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L21">
-        <v>6</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N21">
-        <v>9</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P21" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1">
-        <v>288</v>
-      </c>
-      <c r="C22" s="3">
-        <v>45073</v>
-      </c>
-      <c r="D22" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E22" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0288/01</v>
-      </c>
-      <c r="G22" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F22),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>8d61f76a-54b3-49fb-8bf4-760705670b34</v>
-      </c>
-      <c r="H22" s="5">
-        <v>1</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J22" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="L22">
-        <v>6</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="N22">
-        <v>9</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P22" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1">
-        <v>20</v>
-      </c>
-      <c r="C23" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D23" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E23" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0020/06</v>
-      </c>
-      <c r="G23" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F23),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>6378cec2-a21f-4de6-bbfe-d9fd0835362b</v>
-      </c>
-      <c r="H23" s="5">
-        <v>6</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J23" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L23">
-        <v>9</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N23" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P23" t="s">
-        <v>2287</v>
-      </c>
-      <c r="Q23" s="2"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1">
-        <v>86</v>
-      </c>
-      <c r="C24" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D24" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E24" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0086/01</v>
-      </c>
-      <c r="G24" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F24),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>74d14da7-190a-4785-b3ec-6a521b23b645</v>
-      </c>
-      <c r="H24" s="5">
-        <v>1</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J24" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L24">
-        <v>9</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N24" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P24" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" s="1">
-        <v>188</v>
-      </c>
-      <c r="C25" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D25" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E25" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F25" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0188/01</v>
-      </c>
-      <c r="G25" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F25),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>ab85fe92-97f7-4826-ab50-5c0b9e814528</v>
-      </c>
-      <c r="H25" s="5">
-        <v>1</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J25" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L25">
-        <v>9</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N25" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P25" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1">
-        <v>198</v>
-      </c>
-      <c r="C26" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D26" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E26" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0198/01</v>
-      </c>
-      <c r="G26" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F26),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>5ad12bac-9cc8-4b1f-a09b-8ee41fee634d</v>
-      </c>
-      <c r="H26" s="5">
-        <v>1</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J26" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L26">
-        <v>9</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N26" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P26" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" s="1">
-        <v>199</v>
-      </c>
-      <c r="C27" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D27" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E27" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F27" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0199/01</v>
-      </c>
-      <c r="G27" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F27),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>c565827a-cbc8-4b0f-ab3f-4e1310efff3f</v>
-      </c>
-      <c r="H27" s="5">
-        <v>1</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J27" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L27">
-        <v>9</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N27" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P27" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" s="1">
-        <v>204</v>
-      </c>
-      <c r="C28" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D28" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E28" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F28" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0204/01</v>
-      </c>
-      <c r="G28" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F28),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>d5538f57-d026-49ad-bb63-f2d9f1372647</v>
-      </c>
-      <c r="H28" s="5">
-        <v>1</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J28" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L28">
-        <v>9</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N28" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O28" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P28" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" s="1">
-        <v>207</v>
-      </c>
-      <c r="C29" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D29" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E29" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F29" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0207/02</v>
-      </c>
-      <c r="G29" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F29),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>284bf907-db91-4f81-b1cd-b837b6cae91f</v>
-      </c>
-      <c r="H29" s="5">
-        <v>2</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J29" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L29">
-        <v>9</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N29" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P29" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" s="1">
-        <v>209</v>
-      </c>
-      <c r="C30" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D30" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E30" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F30" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0209/01</v>
-      </c>
-      <c r="G30" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F30),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>0a0b3138-0ce0-4e10-a0a5-68fe1bbecd80</v>
-      </c>
-      <c r="H30" s="5">
-        <v>1</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J30" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L30">
-        <v>9</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N30" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P30" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>29</v>
-      </c>
-      <c r="B31" s="1">
-        <v>269</v>
-      </c>
-      <c r="C31" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D31" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E31" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F31" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0269/01</v>
-      </c>
-      <c r="G31" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F31),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>3a7f1148-3157-4426-8a96-f391a973cfdc</v>
-      </c>
-      <c r="H31" s="5">
-        <v>1</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J31" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L31">
-        <v>9</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N31" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P31" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>30</v>
-      </c>
-      <c r="B32" s="1">
-        <v>237</v>
-      </c>
-      <c r="C32" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D32" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E32" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F32" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0237/01</v>
-      </c>
-      <c r="G32" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F32),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>51e016ed-4d50-4b5d-ba7b-030e509d1cc1</v>
-      </c>
-      <c r="H32" s="5">
-        <v>1</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J32" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L32">
-        <v>9</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N32" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O32" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P32" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>31</v>
-      </c>
-      <c r="B33" s="1">
-        <v>136</v>
-      </c>
-      <c r="C33" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D33" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E33" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>0136/01</v>
-      </c>
-      <c r="G33" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F33),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>246d347e-03ba-4e56-999a-3c5200df65c0</v>
-      </c>
-      <c r="H33" s="5">
-        <v>1</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J33" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L33">
-        <v>9</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N33" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P33" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>32</v>
-      </c>
-      <c r="B34" s="1">
-        <v>175</v>
-      </c>
-      <c r="C34" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D34" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E34" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F34" s="2" t="str">
-        <f t="shared" ref="F34:F46" si="1">CONCATENATE(TEXT(B34,"0000"),"/",TEXT(H34,"00"))</f>
-        <v>0175/02</v>
-      </c>
-      <c r="G34" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F34),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>c2dbbaf4-a305-4cc0-9a02-2611482b3406</v>
-      </c>
-      <c r="H34" s="5">
-        <v>2</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J34" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L34">
-        <v>9</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N34" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P34" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>33</v>
-      </c>
-      <c r="B35" s="1">
-        <v>91</v>
-      </c>
-      <c r="C35" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D35" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E35" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F35" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0091/02</v>
-      </c>
-      <c r="G35" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F35),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>4eeca9af-7306-44a1-b09e-f8d9602ef42d</v>
-      </c>
-      <c r="H35" s="5">
-        <v>2</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J35" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L35">
-        <v>9</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N35" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O35" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P35" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>34</v>
-      </c>
-      <c r="B36" s="1">
-        <v>35</v>
-      </c>
-      <c r="C36" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D36" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E36" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F36" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0035/01</v>
-      </c>
-      <c r="G36" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F36),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>17faf95b-7092-4ba0-a5bf-b51592288efa</v>
-      </c>
-      <c r="H36" s="5">
-        <v>1</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J36" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L36">
-        <v>9</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N36" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O36" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P36" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>35</v>
-      </c>
-      <c r="B37" s="1">
-        <v>30</v>
-      </c>
-      <c r="C37" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D37" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E37" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F37" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0030/01</v>
-      </c>
-      <c r="G37" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F37),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>49e86705-aef0-4425-b0a1-87c63a48a9df</v>
-      </c>
-      <c r="H37" s="5">
-        <v>1</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J37" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L37">
-        <v>9</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N37" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P37" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>36</v>
-      </c>
-      <c r="B38" s="1">
-        <v>223</v>
-      </c>
-      <c r="C38" s="3">
-        <v>45068</v>
-      </c>
-      <c r="D38" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E38" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F38" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0223/01</v>
-      </c>
-      <c r="G38" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F38),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>1120759b-420d-4498-a9e3-8eee7a4aa6a3</v>
-      </c>
-      <c r="H38" s="5">
-        <v>1</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J38" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L38">
-        <v>9</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N38" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O38" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P38" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>37</v>
-      </c>
-      <c r="B39" s="1">
-        <v>210</v>
-      </c>
-      <c r="C39" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D39" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E39" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F39" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0210/01</v>
-      </c>
-      <c r="G39" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F39),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>99e4457f-dc39-440d-9b81-7a19994aff4f</v>
-      </c>
-      <c r="H39" s="5">
-        <v>1</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J39" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L39">
-        <v>9</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N39" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O39" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P39" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>38</v>
-      </c>
-      <c r="B40" s="1">
-        <v>203</v>
-      </c>
-      <c r="C40" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D40" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E40" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F40" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0203/02</v>
-      </c>
-      <c r="G40" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F40),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>6a249484-3f24-4f32-b846-1dc828dd6187</v>
-      </c>
-      <c r="H40" s="5">
-        <v>2</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J40" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L40">
-        <v>9</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N40" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O40" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P40" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>39</v>
-      </c>
-      <c r="B41" s="1">
-        <v>173</v>
-      </c>
-      <c r="C41" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D41" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E41" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F41" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0173/01</v>
-      </c>
-      <c r="G41" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F41),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>2e445697-e499-490b-ba40-6ab9412e82d0</v>
-      </c>
-      <c r="H41" s="5">
-        <v>1</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J41" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L41">
-        <v>9</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N41" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O41" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P41" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>40</v>
-      </c>
-      <c r="B42" s="1">
-        <v>70</v>
-      </c>
-      <c r="C42" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D42" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E42" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F42" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0070/02</v>
-      </c>
-      <c r="G42" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F42),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>e069d11c-5e65-4ba3-ba65-8bc1adce2860</v>
-      </c>
-      <c r="H42" s="5">
-        <v>2</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J42" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L42">
-        <v>9</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N42" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O42" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P42" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>41</v>
-      </c>
-      <c r="B43" s="1">
-        <v>220</v>
-      </c>
-      <c r="C43" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D43" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E43" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F43" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0220/01</v>
-      </c>
-      <c r="G43" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F43),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>e2323cc1-4e59-4fb6-b892-e52d886244c9</v>
-      </c>
-      <c r="H43" s="5">
-        <v>1</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J43" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L43">
-        <v>9</v>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N43" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O43" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P43" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>42</v>
-      </c>
-      <c r="B44" s="1">
-        <v>240</v>
-      </c>
-      <c r="C44" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D44" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E44" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F44" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0240/04</v>
-      </c>
-      <c r="G44" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F44),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>9cbb9717-8f39-4d89-964f-344e577c59ec</v>
-      </c>
-      <c r="H44" s="5">
-        <v>4</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J44" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L44">
-        <v>9</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N44" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O44" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P44" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>43</v>
-      </c>
-      <c r="B45" s="1">
-        <v>283</v>
-      </c>
-      <c r="C45" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D45" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E45" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F45" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0283/01</v>
-      </c>
-      <c r="G45" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F45),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>f8c71a6e-498f-40e4-a971-865a2bad5eb4</v>
-      </c>
-      <c r="H45" s="5">
-        <v>1</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J45" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L45">
-        <v>9</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N45" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O45" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P45" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>44</v>
-      </c>
-      <c r="B46" s="1">
-        <v>295</v>
-      </c>
-      <c r="C46" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D46" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E46" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F46" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>0295/01</v>
-      </c>
-      <c r="G46" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F46),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>7d824e1d-9db7-4658-a783-9fab5f93fffc</v>
-      </c>
-      <c r="H46" s="5">
-        <v>1</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J46" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L46">
-        <v>9</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N46" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O46" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P46" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>45</v>
-      </c>
-      <c r="B47" s="1">
-        <v>212</v>
-      </c>
-      <c r="C47" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D47" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E47" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F47" s="2" t="str">
-        <f t="shared" ref="F47:F86" si="2">CONCATENATE(TEXT(B47,"0000"),"/",TEXT(H47,"00"))</f>
-        <v>0212/01</v>
-      </c>
-      <c r="G47" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F47),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>bdbb921c-ba84-4a1e-9cf6-4e10fab7e2fe</v>
-      </c>
-      <c r="H47" s="5">
-        <v>1</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J47" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L47">
-        <v>9</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N47" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O47" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P47" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>46</v>
-      </c>
-      <c r="B48" s="1">
-        <v>301</v>
-      </c>
-      <c r="C48" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D48" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E48" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F48" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0301/01</v>
-      </c>
-      <c r="G48" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F48),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>1ab440ce-f136-4a23-99b4-693c02499e9d</v>
-      </c>
-      <c r="H48" s="5">
-        <v>1</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J48" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L48">
-        <v>9</v>
-      </c>
-      <c r="M48" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N48" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O48" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P48" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>47</v>
-      </c>
-      <c r="B49" s="1">
-        <v>270</v>
-      </c>
-      <c r="C49" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D49" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E49" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F49" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0270/01</v>
-      </c>
-      <c r="G49" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F49),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>bc3a3da3-a441-4ce9-a5bb-0ba8c127a425</v>
-      </c>
-      <c r="H49" s="5">
-        <v>1</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J49" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L49">
-        <v>9</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N49" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P49" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>48</v>
-      </c>
-      <c r="B50" s="1">
-        <v>271</v>
-      </c>
-      <c r="C50" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D50" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E50" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F50" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0271/07</v>
-      </c>
-      <c r="G50" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F50),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>f5d5b342-025f-4b39-a4c2-f00cd85cc0cb</v>
-      </c>
-      <c r="H50" s="5">
-        <v>7</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J50" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L50">
-        <v>9</v>
-      </c>
-      <c r="M50" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N50" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O50" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P50" t="s">
-        <v>2287</v>
-      </c>
-      <c r="Q50" s="2"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>49</v>
-      </c>
-      <c r="B51" s="1">
-        <v>273</v>
-      </c>
-      <c r="C51" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D51" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E51" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F51" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0273/01</v>
-      </c>
-      <c r="G51" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F51),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>7bebcada-dc4e-41c8-85f0-f2a9fede4d4a</v>
-      </c>
-      <c r="H51" s="5">
-        <v>1</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J51" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L51">
-        <v>9</v>
-      </c>
-      <c r="M51" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N51" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O51" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P51" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>50</v>
-      </c>
-      <c r="B52" s="1">
-        <v>274</v>
-      </c>
-      <c r="C52" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D52" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E52" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F52" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0274/01</v>
-      </c>
-      <c r="G52" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F52),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>131ed2bb-bd88-4077-b3c7-1cc180f25318</v>
-      </c>
-      <c r="H52" s="5">
-        <v>1</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J52" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L52">
-        <v>9</v>
-      </c>
-      <c r="M52" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N52" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O52" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P52" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>51</v>
-      </c>
-      <c r="B53" s="1">
-        <v>276</v>
-      </c>
-      <c r="C53" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D53" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E53" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F53" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0276/01</v>
-      </c>
-      <c r="G53" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F53),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>ab5cd0ef-ec0e-4de4-95ef-27459353c94a</v>
-      </c>
-      <c r="H53" s="5">
-        <v>1</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J53" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L53">
-        <v>9</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N53" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O53" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P53" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>52</v>
-      </c>
-      <c r="B54" s="1">
-        <v>279</v>
-      </c>
-      <c r="C54" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D54" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E54" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F54" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0279/01</v>
-      </c>
-      <c r="G54" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F54),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>46a58977-24bb-4ff8-bf6d-387701362cd3</v>
-      </c>
-      <c r="H54" s="5">
-        <v>1</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J54" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L54">
-        <v>9</v>
-      </c>
-      <c r="M54" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N54" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O54" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P54" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>53</v>
-      </c>
-      <c r="B55" s="1">
-        <v>298</v>
-      </c>
-      <c r="C55" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D55" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E55" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F55" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0298/01</v>
-      </c>
-      <c r="G55" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F55),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>93a5aba7-7493-4eac-bd7a-55f3ba79ca45</v>
-      </c>
-      <c r="H55" s="5">
-        <v>1</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J55" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L55">
-        <v>9</v>
-      </c>
-      <c r="M55" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N55" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O55" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P55" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>54</v>
-      </c>
-      <c r="B56" s="1">
-        <v>299</v>
-      </c>
-      <c r="C56" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D56" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E56" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F56" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0299/01</v>
-      </c>
-      <c r="G56" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F56),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>231f4ecd-9597-40e8-abaa-eac824a97eaf</v>
-      </c>
-      <c r="H56" s="5">
-        <v>1</v>
-      </c>
-      <c r="I56" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J56" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L56">
-        <v>9</v>
-      </c>
-      <c r="M56" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N56" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O56" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P56" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>55</v>
-      </c>
-      <c r="B57" s="1">
-        <v>303</v>
-      </c>
-      <c r="C57" s="3">
-        <v>45068</v>
-      </c>
-      <c r="D57" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E57" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F57" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0303/02</v>
-      </c>
-      <c r="G57" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F57),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>8132f5b2-1107-47d4-bb34-91456c2ff343</v>
-      </c>
-      <c r="H57" s="5">
-        <v>2</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J57" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L57">
-        <v>9</v>
-      </c>
-      <c r="M57" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N57" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O57" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P57" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>56</v>
-      </c>
-      <c r="B58" s="1">
-        <v>305</v>
-      </c>
-      <c r="C58" s="3">
-        <v>45068</v>
-      </c>
-      <c r="D58" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E58" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F58" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0305/01</v>
-      </c>
-      <c r="G58" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F58),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>26ee102d-37f2-4be5-9e88-959b8c1666d7</v>
-      </c>
-      <c r="H58" s="5">
-        <v>1</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J58" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L58">
-        <v>9</v>
-      </c>
-      <c r="M58" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N58" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O58" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P58" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>57</v>
-      </c>
-      <c r="B59" s="1">
-        <v>242</v>
-      </c>
-      <c r="C59" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D59" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E59" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F59" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0242/01</v>
-      </c>
-      <c r="G59" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F59),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>887e37fd-dac2-42e9-abfe-d473e9bf7afd</v>
-      </c>
-      <c r="H59" s="5">
-        <v>1</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J59" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K59" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L59">
-        <v>9</v>
-      </c>
-      <c r="M59" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N59" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O59" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P59" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>58</v>
-      </c>
-      <c r="B60" s="1">
-        <v>241</v>
-      </c>
-      <c r="C60" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D60" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E60" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F60" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0241/01</v>
-      </c>
-      <c r="G60" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F60),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>01886405-7fd7-4ecf-9c0d-e729aa3e824d</v>
-      </c>
-      <c r="H60" s="5">
-        <v>1</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J60" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K60" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L60">
-        <v>9</v>
-      </c>
-      <c r="M60" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N60" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O60" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P60" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>59</v>
-      </c>
-      <c r="B61" s="1">
-        <v>244</v>
-      </c>
-      <c r="C61" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D61" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E61" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F61" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0244/05</v>
-      </c>
-      <c r="G61" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F61),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>4e009639-9d82-446c-9dd3-ae9891d51f75</v>
-      </c>
-      <c r="H61" s="5">
-        <v>5</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J61" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K61" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L61">
-        <v>9</v>
-      </c>
-      <c r="M61" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N61" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O61" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P61" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>60</v>
-      </c>
-      <c r="B62" s="1">
-        <v>246</v>
-      </c>
-      <c r="C62" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D62" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E62" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F62" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0246/01</v>
-      </c>
-      <c r="G62" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F62),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>dc9d42f9-e2ae-4cb4-b4e2-742e37f2a355</v>
-      </c>
-      <c r="H62" s="5">
-        <v>1</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J62" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K62" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L62">
-        <v>9</v>
-      </c>
-      <c r="M62" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N62" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O62" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P62" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>61</v>
-      </c>
-      <c r="B63" s="1">
-        <v>257</v>
-      </c>
-      <c r="C63" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D63" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E63" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F63" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0257/01</v>
-      </c>
-      <c r="G63" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F63),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>f42941d7-e985-4f40-a421-2b382ea69f20</v>
-      </c>
-      <c r="H63" s="5">
-        <v>1</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J63" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K63" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L63">
-        <v>9</v>
-      </c>
-      <c r="M63" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N63" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O63" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P63" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>62</v>
-      </c>
-      <c r="B64" s="1">
-        <v>258</v>
-      </c>
-      <c r="C64" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D64" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E64" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F64" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0258/01</v>
-      </c>
-      <c r="G64" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F64),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>3f4ad135-280b-4d39-8dd7-a1eaa09a6f65</v>
-      </c>
-      <c r="H64" s="5">
-        <v>1</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J64" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K64" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L64">
-        <v>9</v>
-      </c>
-      <c r="M64" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N64" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O64" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P64" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>63</v>
-      </c>
-      <c r="B65" s="1">
-        <v>260</v>
-      </c>
-      <c r="C65" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D65" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E65" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F65" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0260/01</v>
-      </c>
-      <c r="G65" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F65),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>1e98d195-38fa-4cee-9e2b-8731c2d972a9</v>
-      </c>
-      <c r="H65" s="5">
-        <v>1</v>
-      </c>
-      <c r="I65" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J65" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K65" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L65">
-        <v>9</v>
-      </c>
-      <c r="M65" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N65" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O65" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P65" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>64</v>
-      </c>
-      <c r="B66" s="1">
-        <v>11</v>
-      </c>
-      <c r="C66" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D66" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E66" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F66" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0011/01</v>
-      </c>
-      <c r="G66" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F66),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>2ccea0b9-3189-42f5-b9ac-bf2de4c8b9d1</v>
-      </c>
-      <c r="H66" s="5">
-        <v>1</v>
-      </c>
-      <c r="I66" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J66" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K66" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L66">
-        <v>9</v>
-      </c>
-      <c r="M66" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N66" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O66" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P66" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>65</v>
-      </c>
-      <c r="B67" s="1">
-        <v>54</v>
-      </c>
-      <c r="C67" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D67" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E67" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F67" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0054/01</v>
-      </c>
-      <c r="G67" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F67),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>251a6b1c-cb31-4714-842b-08a70b8d8e45</v>
-      </c>
-      <c r="H67" s="5">
-        <v>1</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J67" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K67" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L67">
-        <v>9</v>
-      </c>
-      <c r="M67" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N67" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O67" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P67" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>66</v>
-      </c>
-      <c r="B68" s="1">
-        <v>55</v>
-      </c>
-      <c r="C68" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D68" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E68" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F68" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0055/01</v>
-      </c>
-      <c r="G68" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F68),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>7259feb6-0f98-4889-94cb-f659c3370439</v>
-      </c>
-      <c r="H68" s="5">
-        <v>1</v>
-      </c>
-      <c r="I68" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J68" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K68" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L68">
-        <v>9</v>
-      </c>
-      <c r="M68" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N68" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O68" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P68" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>67</v>
-      </c>
-      <c r="B69" s="1">
-        <v>94</v>
-      </c>
-      <c r="C69" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D69" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E69" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F69" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0094/01</v>
-      </c>
-      <c r="G69" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F69),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>bfc5c348-7507-41cc-b9fc-705307b9188e</v>
-      </c>
-      <c r="H69" s="5">
-        <v>1</v>
-      </c>
-      <c r="I69" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J69" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K69" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L69">
-        <v>9</v>
-      </c>
-      <c r="M69" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N69" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O69" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P69" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>68</v>
-      </c>
-      <c r="B70" s="1">
-        <v>197</v>
-      </c>
-      <c r="C70" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D70" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E70" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F70" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0197/01</v>
-      </c>
-      <c r="G70" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F70),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>a02e50f2-dff3-4407-9f7c-cbeda3881e87</v>
-      </c>
-      <c r="H70" s="5">
-        <v>1</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J70" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L70">
-        <v>9</v>
-      </c>
-      <c r="M70" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N70" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O70" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P70" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>69</v>
-      </c>
-      <c r="B71" s="1">
-        <v>206</v>
-      </c>
-      <c r="C71" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D71" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E71" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F71" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0206/01</v>
-      </c>
-      <c r="G71" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F71),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>3b95bfb2-5ee3-4fd9-84b7-5aa8b9297a09</v>
-      </c>
-      <c r="H71" s="5">
-        <v>1</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J71" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K71" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L71">
-        <v>9</v>
-      </c>
-      <c r="M71" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N71" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O71" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P71" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>70</v>
-      </c>
-      <c r="B72" s="1">
-        <v>227</v>
-      </c>
-      <c r="C72" s="3">
-        <v>45072</v>
-      </c>
-      <c r="D72" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E72" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F72" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0227/01</v>
-      </c>
-      <c r="G72" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F72),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>1d646d71-792c-4dd9-a126-f2a92f710399</v>
-      </c>
-      <c r="H72" s="5">
-        <v>1</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J72" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L72">
-        <v>9</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N72" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O72" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P72" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>71</v>
-      </c>
-      <c r="B73" s="1">
-        <v>232</v>
-      </c>
-      <c r="C73" s="3">
-        <v>45073</v>
-      </c>
-      <c r="D73" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E73" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F73" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0232/02</v>
-      </c>
-      <c r="G73" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F73),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>32e8416c-5bd7-4fe5-bdb9-a03e7278ccd6</v>
-      </c>
-      <c r="H73" s="5">
-        <v>2</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J73" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L73">
-        <v>9</v>
-      </c>
-      <c r="M73" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N73" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O73" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P73" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>72</v>
-      </c>
-      <c r="B74" s="1">
-        <v>12</v>
-      </c>
-      <c r="C74" s="3">
-        <v>45064</v>
-      </c>
-      <c r="D74" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E74" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F74" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0012/01</v>
-      </c>
-      <c r="G74" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F74),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>a614e163-4d87-4c50-8f3b-e0f3cf9b767e</v>
-      </c>
-      <c r="H74" s="5">
-        <v>1</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J74" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L74">
-        <v>9</v>
-      </c>
-      <c r="M74" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N74" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O74" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P74" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>73</v>
-      </c>
-      <c r="B75" s="1">
-        <v>23</v>
-      </c>
-      <c r="C75" s="3">
-        <v>45064</v>
-      </c>
-      <c r="D75" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E75" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F75" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0023/01</v>
-      </c>
-      <c r="G75" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F75),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>084bdf27-4247-4d93-bcb8-f623739e1472</v>
-      </c>
-      <c r="H75" s="5">
-        <v>1</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J75" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L75">
-        <v>9</v>
-      </c>
-      <c r="M75" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N75" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O75" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P75" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>74</v>
-      </c>
-      <c r="B76" s="1">
-        <v>38</v>
-      </c>
-      <c r="C76" s="3">
-        <v>45064</v>
-      </c>
-      <c r="D76" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E76" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F76" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0038/01</v>
-      </c>
-      <c r="G76" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F76),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>246fe843-e2ed-46b1-a54a-8f98167dead4</v>
-      </c>
-      <c r="H76" s="5">
-        <v>1</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J76" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K76" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L76">
-        <v>9</v>
-      </c>
-      <c r="M76" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N76" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O76" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P76" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>75</v>
-      </c>
-      <c r="B77" s="1">
-        <v>59</v>
-      </c>
-      <c r="C77" s="3">
-        <v>45064</v>
-      </c>
-      <c r="D77" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E77" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F77" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0059/01</v>
-      </c>
-      <c r="G77" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F77),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>67434fb5-9f39-409c-9faf-033ed565807a</v>
-      </c>
-      <c r="H77" s="5">
-        <v>1</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J77" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K77" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L77">
-        <v>9</v>
-      </c>
-      <c r="M77" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N77" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O77" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P77" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>76</v>
-      </c>
-      <c r="B78" s="1">
-        <v>118</v>
-      </c>
-      <c r="C78" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D78" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E78" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F78" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0118/01</v>
-      </c>
-      <c r="G78" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F78),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>3f12c656-f3fe-432d-80f7-c7a7ecd44930</v>
-      </c>
-      <c r="H78" s="5">
-        <v>1</v>
-      </c>
-      <c r="I78" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J78" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K78" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L78">
-        <v>9</v>
-      </c>
-      <c r="M78" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N78" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O78" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P78" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>77</v>
-      </c>
-      <c r="B79" s="1">
-        <v>150</v>
-      </c>
-      <c r="C79" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D79" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E79" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F79" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0150/01</v>
-      </c>
-      <c r="G79" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F79),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>badc7349-8abc-48bf-b4ab-c350185ad38e</v>
-      </c>
-      <c r="H79" s="5">
-        <v>1</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J79" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K79" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L79">
-        <v>9</v>
-      </c>
-      <c r="M79" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N79" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O79" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P79" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>78</v>
-      </c>
-      <c r="B80" s="1">
-        <v>156</v>
-      </c>
-      <c r="C80" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D80" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E80" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F80" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0156/01</v>
-      </c>
-      <c r="G80" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F80),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>453b864e-7cea-4c0b-9452-df577c602605</v>
-      </c>
-      <c r="H80" s="5">
-        <v>1</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J80" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K80" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L80">
-        <v>9</v>
-      </c>
-      <c r="M80" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N80" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O80" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P80" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>79</v>
-      </c>
-      <c r="B81" s="1">
-        <v>158</v>
-      </c>
-      <c r="C81" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D81" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E81" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F81" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0158/01</v>
-      </c>
-      <c r="G81" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F81),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>1a97bb54-85ce-44c3-815a-933a2c22e2b6</v>
-      </c>
-      <c r="H81" s="5">
-        <v>1</v>
-      </c>
-      <c r="I81" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J81" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K81" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L81">
-        <v>9</v>
-      </c>
-      <c r="M81" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N81" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O81" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P81" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>80</v>
-      </c>
-      <c r="B82" s="1">
-        <v>181</v>
-      </c>
-      <c r="C82" s="3">
-        <v>45066</v>
-      </c>
-      <c r="D82" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E82" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F82" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0181/01</v>
-      </c>
-      <c r="G82" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F82),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>0ede2acc-58ff-4d08-b5fd-fd61f3961b31</v>
-      </c>
-      <c r="H82" s="5">
-        <v>1</v>
-      </c>
-      <c r="I82" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J82" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K82" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L82">
-        <v>9</v>
-      </c>
-      <c r="M82" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N82" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O82" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P82" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>81</v>
-      </c>
-      <c r="B83" s="1">
-        <v>161</v>
-      </c>
-      <c r="C83" s="3">
-        <v>45071</v>
-      </c>
-      <c r="D83" t="s">
-        <v>2247</v>
-      </c>
-      <c r="E83" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F83" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0161/01</v>
-      </c>
-      <c r="G83" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F83),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>cdc02bb3-99b6-46c5-854e-a9ef1fb729fc</v>
-      </c>
-      <c r="H83" s="5">
-        <v>1</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>2288</v>
-      </c>
-      <c r="J83" t="s">
-        <v>2287</v>
-      </c>
-      <c r="K83" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L83">
-        <v>9</v>
-      </c>
-      <c r="M83" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N83" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O83" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P83" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>82</v>
-      </c>
-      <c r="B84" s="1">
-        <v>265</v>
-      </c>
-      <c r="C84" s="3">
-        <v>45068</v>
-      </c>
-      <c r="D84" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E84" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F84" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0265/02</v>
-      </c>
-      <c r="G84" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F84),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>2bd6129c-7a32-4378-bdc1-0081eebbb548</v>
-      </c>
-      <c r="H84" s="5">
-        <v>2</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="J84">
-        <v>6</v>
-      </c>
-      <c r="K84" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L84">
-        <v>9</v>
-      </c>
-      <c r="M84" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N84" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O84" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P84" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>83</v>
-      </c>
-      <c r="B85" s="1">
-        <v>259</v>
-      </c>
-      <c r="C85" s="3">
-        <v>45065</v>
-      </c>
-      <c r="D85" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E85" t="s">
-        <v>2250</v>
-      </c>
-      <c r="F85" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0259/01</v>
-      </c>
-      <c r="G85" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F85),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>9077e47a-4b5a-4279-94de-53302d508f27</v>
-      </c>
-      <c r="H85" s="5">
-        <v>1</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="J85">
-        <v>6</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L85">
-        <v>9</v>
-      </c>
-      <c r="M85" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N85" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O85" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P85" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>84</v>
-      </c>
-      <c r="B86" s="1">
-        <v>293</v>
-      </c>
-      <c r="C86" s="3">
-        <v>45075</v>
-      </c>
-      <c r="D86" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E86" t="s">
-        <v>2250</v>
-      </c>
-      <c r="F86" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>0293/01</v>
-      </c>
-      <c r="G86" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F86),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>89a059a2-2cfb-484b-8a95-1eb9de9bf706</v>
-      </c>
-      <c r="H86" s="5">
-        <v>1</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>2285</v>
-      </c>
-      <c r="J86">
-        <v>6</v>
-      </c>
-      <c r="K86" s="2" t="s">
-        <v>2286</v>
-      </c>
-      <c r="L86">
-        <v>9</v>
-      </c>
-      <c r="M86" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="N86" t="s">
-        <v>2287</v>
-      </c>
-      <c r="O86" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="P86" t="s">
-        <v>2287</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:P86" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}"/>
+  <autoFilter ref="A1:P4" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
@@ -11828,7 +7560,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I1 K1:K2 I100:I1048576 K100:K1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="I1 K1:K2 I18:I1048576 K18:K1048576" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
implementación de clases en el formulario 06
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80987834-2A1C-4F89-8B5C-372C09E0C550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646E9083-5497-4577-8BE1-114B7FFF3516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
@@ -20,26 +20,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$M$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$B$1134</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2386" uniqueCount="2297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2472" uniqueCount="2337">
   <si>
     <t>Hogar</t>
   </si>
@@ -6923,13 +6914,133 @@
     <t>01</t>
   </si>
   <si>
+    <t>03 04</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0312/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0313/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0313/02</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0314/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0314/02</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0315/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0316/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0316/02</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0317/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0317/02</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0318/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0319/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0319/02</t>
+  </si>
+  <si>
+    <t>e78059c6-5c13-4937-b91e-b1c2128cf08b</t>
+  </si>
+  <si>
+    <t>d7fb77ad-cda7-4421-922d-c49c40788e86</t>
+  </si>
+  <si>
+    <t>79eb627a-37a2-4ebf-991c-9866a068da02</t>
+  </si>
+  <si>
+    <t>c362ca4b-72cf-44df-aca0-51bb0df79ff1</t>
+  </si>
+  <si>
+    <t>467db9fa-77dc-4fff-a3c4-408068e58f35</t>
+  </si>
+  <si>
+    <t>f1479827-ccfd-4330-b0b7-3dab8b9b38e3</t>
+  </si>
+  <si>
+    <t>b4931c2a-b13a-4f76-967d-e455dadcc0ad</t>
+  </si>
+  <si>
+    <t>1cf94c97-30a4-4e99-823e-37faeebad529</t>
+  </si>
+  <si>
+    <t>261bb2c1-fb60-4add-bc34-5093e2e08613</t>
+  </si>
+  <si>
+    <t>4c22d313-e4f2-4382-984a-5349332b6d77</t>
+  </si>
+  <si>
+    <t>bab3d934-a1ba-4a15-9e6f-f707a8c2a76c</t>
+  </si>
+  <si>
+    <t>2b584d49-5614-4f69-9207-8975a551d7af</t>
+  </si>
+  <si>
+    <t>b572048a-fde5-4882-8b63-c82cd596227c</t>
+  </si>
+  <si>
     <t>02</t>
   </si>
   <si>
+    <t>2.4</t>
+  </si>
+  <si>
     <t>9</t>
   </si>
   <si>
-    <t>Visita regular En el hogar</t>
+    <t>03 04 06 07 08</t>
+  </si>
+  <si>
+    <t>03 04 06</t>
+  </si>
+  <si>
+    <t>04 02 05 03</t>
+  </si>
+  <si>
+    <t>03 05 08</t>
+  </si>
+  <si>
+    <t>02 03 04</t>
+  </si>
+  <si>
+    <t>03 08</t>
+  </si>
+  <si>
+    <t>04 05</t>
+  </si>
+  <si>
+    <t>02 05 06</t>
+  </si>
+  <si>
+    <t>04 07</t>
+  </si>
+  <si>
+    <t>03 04 05</t>
+  </si>
+  <si>
+    <t>02 03</t>
+  </si>
+  <si>
+    <t>03 06</t>
   </si>
 </sst>
 </file>
@@ -7329,10 +7440,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7340,11 +7451,12 @@
     <col min="2" max="2" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="38.28515625" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="5"/>
-    <col min="9" max="13" width="11.42578125" style="2"/>
+    <col min="9" max="10" width="11.42578125" style="2" customWidth="1"/>
+    <col min="11" max="13" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -7393,10 +7505,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C2" s="3">
-        <v>45084</v>
+        <v>45098</v>
       </c>
       <c r="D2" t="s">
         <v>2244</v>
@@ -7406,23 +7518,23 @@
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F4" si="0">CONCATENATE(TEXT(B2,"0000"),"/",TEXT(H2,"00"))</f>
-        <v>0113/01</v>
+        <v>0120/01</v>
       </c>
       <c r="G2" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F2),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>381f3c56-41de-48c1-b3ea-275bcf33c389</v>
+        <v>fe6cff7a-cd86-4d43-9df4-814b7f8897c7</v>
       </c>
       <c r="H2" s="5">
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>2287</v>
-      </c>
-      <c r="J2" s="2">
-        <v>9</v>
+        <v>2291</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2291</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>2293</v>
+        <v>2322</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>2290</v>
@@ -7436,10 +7548,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>66</v>
+        <v>265</v>
       </c>
       <c r="C3" s="3">
-        <v>45083</v>
+        <v>45090</v>
       </c>
       <c r="D3" t="s">
         <v>2244</v>
@@ -7449,23 +7561,23 @@
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
-        <v>0066/01</v>
+        <v>0265/02</v>
       </c>
       <c r="G3" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F3),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>ba17ac69-724c-4f09-bb9d-e72f5302aa46</v>
+        <v>2bd6129c-7a32-4378-bdc1-0081eebbb548</v>
       </c>
       <c r="H3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>2287</v>
+        <v>2291</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>2295</v>
+        <v>2291</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>2293</v>
+        <v>2322</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>2290</v>
@@ -7479,10 +7591,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>275</v>
+        <v>117</v>
       </c>
       <c r="C4" s="3">
-        <v>45078</v>
+        <v>45097</v>
       </c>
       <c r="D4" t="s">
         <v>2244</v>
@@ -7492,20 +7604,20 @@
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>0275/01</v>
+        <v>0117/01</v>
       </c>
       <c r="G4" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F4),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>02e993d3-cc24-4237-a8e5-cf273acff674</v>
+        <v>52f9d29d-a6fa-4a79-a9b0-edd6c7a1a126</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>2287</v>
+        <v>2291</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>2295</v>
+        <v>2291</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>2293</v>
@@ -7522,10 +7634,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>237</v>
+        <v>119</v>
       </c>
       <c r="C5" s="3">
-        <v>45082</v>
+        <v>45100</v>
       </c>
       <c r="D5" t="s">
         <v>2244</v>
@@ -7534,12 +7646,12 @@
         <v>2250</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ref="F5:F17" si="1">CONCATENATE(TEXT(B5,"0000"),"/",TEXT(H5,"00"))</f>
-        <v>0237/01</v>
+        <f t="shared" ref="F5:F16" si="1">CONCATENATE(TEXT(B5,"0000"),"/",TEXT(H5,"00"))</f>
+        <v>0119/01</v>
       </c>
       <c r="G5" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F5),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>51e016ed-4d50-4b5d-ba7b-030e509d1cc1</v>
+        <v>4cff4de7-cf65-4433-8a0d-1534c09e83c9</v>
       </c>
       <c r="H5" s="5">
         <v>1</v>
@@ -7565,24 +7677,24 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>47</v>
+        <v>187</v>
       </c>
       <c r="C6" s="3">
-        <v>45082</v>
+        <v>45097</v>
       </c>
       <c r="D6" t="s">
         <v>2244</v>
       </c>
       <c r="E6" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
-        <v>0047/01</v>
+        <v>0187/01</v>
       </c>
       <c r="G6" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F6),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>7661b3c5-7ff3-403d-9b96-efc931ec943d</v>
+        <v>2bf7ded4-896e-4fd0-a36f-8abd7c5cf317</v>
       </c>
       <c r="H6" s="5">
         <v>1</v>
@@ -7594,7 +7706,7 @@
         <v>2291</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>2293</v>
+        <v>2322</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>2290</v>
@@ -7608,24 +7720,24 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>212</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3">
-        <v>45078</v>
+        <v>45107</v>
       </c>
       <c r="D7" t="s">
         <v>2244</v>
       </c>
       <c r="E7" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
-        <v>0212/01</v>
+        <v>0016/01</v>
       </c>
       <c r="G7" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F7),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>bdbb921c-ba84-4a1e-9cf6-4e10fab7e2fe</v>
+        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
       </c>
       <c r="H7" s="5">
         <v>1</v>
@@ -7637,10 +7749,10 @@
         <v>2291</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>2293</v>
+        <v>2322</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>2290</v>
+        <v>2323</v>
       </c>
       <c r="M7" s="2">
         <v>0</v>
@@ -7651,24 +7763,24 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>242</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3">
-        <v>45078</v>
+        <v>45106</v>
       </c>
       <c r="D8" t="s">
         <v>2244</v>
       </c>
       <c r="E8" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
-        <v>0242/01</v>
+        <v>0016/01</v>
       </c>
       <c r="G8" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F8),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>887e37fd-dac2-42e9-abfe-d473e9bf7afd</v>
+        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
       </c>
       <c r="H8" s="5">
         <v>1</v>
@@ -7680,10 +7792,10 @@
         <v>2291</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>2293</v>
+        <v>2322</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>2290</v>
+        <v>2323</v>
       </c>
       <c r="M8" s="2">
         <v>0</v>
@@ -7694,24 +7806,24 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>205</v>
+        <v>16</v>
       </c>
       <c r="C9" s="3">
-        <v>45078</v>
+        <v>45105</v>
       </c>
       <c r="D9" t="s">
         <v>2244</v>
       </c>
       <c r="E9" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
-        <v>0205/01</v>
+        <v>0016/01</v>
       </c>
       <c r="G9" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F9),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>1845ecd8-25fa-4a6a-9e8b-aa1c4287405d</v>
+        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
       </c>
       <c r="H9" s="5">
         <v>1</v>
@@ -7723,10 +7835,10 @@
         <v>2291</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>2293</v>
+        <v>2322</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>2290</v>
+        <v>2323</v>
       </c>
       <c r="M9" s="2">
         <v>0</v>
@@ -7737,24 +7849,24 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>220</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3">
-        <v>45078</v>
+        <v>45104</v>
       </c>
       <c r="D10" t="s">
         <v>2244</v>
       </c>
       <c r="E10" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
-        <v>0220/01</v>
+        <v>0016/01</v>
       </c>
       <c r="G10" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F10),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>e2323cc1-4e59-4fb6-b892-e52d886244c9</v>
+        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
       </c>
       <c r="H10" s="5">
         <v>1</v>
@@ -7766,10 +7878,10 @@
         <v>2291</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>2293</v>
+        <v>2322</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>2290</v>
+        <v>2323</v>
       </c>
       <c r="M10" s="2">
         <v>0</v>
@@ -7780,24 +7892,24 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>188</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3">
-        <v>45079</v>
+        <v>45103</v>
       </c>
       <c r="D11" t="s">
         <v>2244</v>
       </c>
       <c r="E11" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
-        <v>0188/01</v>
+        <v>0016/01</v>
       </c>
       <c r="G11" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F11),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>ab85fe92-97f7-4826-ab50-5c0b9e814528</v>
+        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
       </c>
       <c r="H11" s="5">
         <v>1</v>
@@ -7809,10 +7921,10 @@
         <v>2291</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>2293</v>
+        <v>2322</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>2290</v>
+        <v>2323</v>
       </c>
       <c r="M11" s="2">
         <v>0</v>
@@ -7823,33 +7935,33 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>199</v>
+        <v>225</v>
       </c>
       <c r="C12" s="3">
-        <v>45083</v>
+        <v>45089</v>
       </c>
       <c r="D12" t="s">
         <v>2244</v>
       </c>
       <c r="E12" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
-        <v>0199/01</v>
+        <v>0225/01</v>
       </c>
       <c r="G12" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F12),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>c565827a-cbc8-4b0f-ab3f-4e1310efff3f</v>
+        <v>1d026f2f-895f-4869-9b6c-ec17624b66fd</v>
       </c>
       <c r="H12" s="5">
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>2291</v>
+        <v>2324</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>2293</v>
@@ -7866,39 +7978,39 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C13" s="3">
-        <v>45084</v>
+        <v>45100</v>
       </c>
       <c r="D13" t="s">
         <v>2244</v>
       </c>
       <c r="E13" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
-        <v>0050/01</v>
+        <v>0016/01</v>
       </c>
       <c r="G13" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F13),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>c784b34a-efc4-4be4-828f-1c1e5dd4d3dd</v>
+        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
       </c>
       <c r="H13" s="5">
         <v>1</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>2291</v>
+        <v>2324</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>2293</v>
+        <v>2322</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>2290</v>
+        <v>2323</v>
       </c>
       <c r="M13" s="2">
         <v>0</v>
@@ -7909,39 +8021,39 @@
         <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" s="3">
-        <v>45084</v>
+        <v>45099</v>
       </c>
       <c r="D14" t="s">
         <v>2244</v>
       </c>
       <c r="E14" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
-        <v>0091/01</v>
+        <v>0090/02</v>
       </c>
       <c r="G14" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F14),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>9634473a-1bf5-44d2-b612-ccb4ac8c9b9b</v>
+        <v>f389fdf6-5f88-437a-a4a4-0ae1f5c736f5</v>
       </c>
       <c r="H14" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>2291</v>
+        <v>2324</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>2293</v>
+        <v>2325</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>2290</v>
+        <v>2323</v>
       </c>
       <c r="M14" s="2">
         <v>0</v>
@@ -7952,39 +8064,39 @@
         <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>148</v>
+        <v>81</v>
       </c>
       <c r="C15" s="3">
-        <v>45082</v>
+        <v>45100</v>
       </c>
       <c r="D15" t="s">
         <v>2244</v>
       </c>
       <c r="E15" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
-        <v>0148/02</v>
+        <v>0081/01</v>
       </c>
       <c r="G15" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F15),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>0298c857-1baf-44cb-8df2-61526b3d622f</v>
+        <v>e34d1792-6830-4820-bcc5-1e89c914e2b9</v>
       </c>
       <c r="H15" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>2291</v>
+        <v>2324</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>2294</v>
+        <v>2326</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>2290</v>
+        <v>2323</v>
       </c>
       <c r="M15" s="2">
         <v>0</v>
@@ -7995,39 +8107,39 @@
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>166</v>
+        <v>59</v>
       </c>
       <c r="C16" s="3">
-        <v>45084</v>
+        <v>45099</v>
       </c>
       <c r="D16" t="s">
         <v>2244</v>
       </c>
       <c r="E16" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
-        <v>0166/02</v>
+        <v>0059/01</v>
       </c>
       <c r="G16" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F16),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>f5da9351-1453-40c3-8f37-b1d8bbfd7600</v>
+        <v>67434fb5-9f39-409c-9faf-033ed565807a</v>
       </c>
       <c r="H16" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>2291</v>
+        <v>2287</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>2291</v>
+        <v>2324</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>2294</v>
+        <v>2327</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>2290</v>
+        <v>2323</v>
       </c>
       <c r="M16" s="2">
         <v>0</v>
@@ -8038,43 +8150,638 @@
         <v>15</v>
       </c>
       <c r="B17" s="1">
-        <v>176</v>
+        <v>70</v>
       </c>
       <c r="C17" s="3">
-        <v>45068</v>
+        <v>45099</v>
       </c>
       <c r="D17" t="s">
-        <v>2296</v>
+        <v>2244</v>
       </c>
       <c r="E17" t="s">
         <v>2245</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="1"/>
-        <v>0176/01</v>
+        <f t="shared" ref="F17:F25" si="2">CONCATENATE(TEXT(B17,"0000"),"/",TEXT(H17,"00"))</f>
+        <v>0070/02</v>
       </c>
       <c r="G17" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F17),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>e96501d6-057d-4e4f-b8e9-46965f3a2e9f</v>
+        <v>e069d11c-5e65-4ba3-ba65-8bc1adce2860</v>
       </c>
       <c r="H17" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>2287</v>
       </c>
       <c r="J17" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>2328</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>2323</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>111</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="2"/>
+        <v>0111/01</v>
+      </c>
+      <c r="G18" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F18),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>c6674d90-1e86-405b-b19c-5a8c0bce0841</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>2329</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>2323</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>49</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45099</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="2"/>
+        <v>0049/05</v>
+      </c>
+      <c r="G19" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F19),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>f1774a4b-b951-4693-8757-467334b011d9</v>
+      </c>
+      <c r="H19" s="5">
+        <v>5</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>2330</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>2323</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>11</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45099</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="2"/>
+        <v>0011/03</v>
+      </c>
+      <c r="G20" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F20),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>d92e77e1-e7fc-4b11-a712-a8f4d651a79d</v>
+      </c>
+      <c r="H20" s="5">
+        <v>3</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>2331</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>2323</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>40</v>
+      </c>
+      <c r="C21" s="3">
+        <v>45100</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="2"/>
+        <v>0040/01</v>
+      </c>
+      <c r="G21" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F21),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>2dfcd22d-1e57-48ae-ab25-338f0960370e</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>2295</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>2291</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>2291</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>2291</v>
-      </c>
+      <c r="L21" s="2" t="s">
+        <v>2323</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1">
+        <v>21</v>
+      </c>
+      <c r="C22" s="3">
+        <v>45099</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="2"/>
+        <v>0021/01</v>
+      </c>
+      <c r="G22" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F22),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>86956ee6-4b03-4a88-8c4e-b83e9df9c8df</v>
+      </c>
+      <c r="H22" s="5">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>2332</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>2323</v>
+      </c>
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>86</v>
+      </c>
+      <c r="C23" s="3">
+        <v>45100</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="2"/>
+        <v>0086/01</v>
+      </c>
+      <c r="G23" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F23),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>74d14da7-190a-4785-b3ec-6a521b23b645</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>2333</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>2323</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>33</v>
+      </c>
+      <c r="C24" s="3">
+        <v>45098</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="2"/>
+        <v>0033/01</v>
+      </c>
+      <c r="G24" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F24),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>a573c7cc-3952-4261-8a03-4b5ecb553281</v>
+      </c>
+      <c r="H24" s="5">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>2334</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>2323</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>105</v>
+      </c>
+      <c r="C25" s="3">
+        <v>45099</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="2"/>
+        <v>0105/01</v>
+      </c>
+      <c r="G25" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F25),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>d3caa522-1d02-465c-83cd-295aaca69a1e</v>
+      </c>
+      <c r="H25" s="5">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>2294</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>2323</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1">
+        <v>134</v>
+      </c>
+      <c r="C26" s="3">
+        <v>45100</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" ref="F26:F27" si="3">CONCATENATE(TEXT(B26,"0000"),"/",TEXT(H26,"00"))</f>
+        <v>0134/01</v>
+      </c>
+      <c r="G26" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F26),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>8f71fa1b-b24c-4648-9cb0-41d5566d1f55</v>
+      </c>
+      <c r="H26" s="5">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>2335</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>2323</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1">
+        <v>24</v>
+      </c>
+      <c r="C27" s="3">
+        <v>45099</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="3"/>
+        <v>0024/01</v>
+      </c>
+      <c r="G27" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F27),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>1e7ab3f1-c9bb-4930-8649-1e5b29241974</v>
+      </c>
+      <c r="H27" s="5">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>2287</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>2336</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>2323</v>
+      </c>
+      <c r="M27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F28"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F29"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F30"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F31"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F33"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F41"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F42"/>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F64"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F65"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F66"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F67"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F68"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F71"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F72"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F73"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F74"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F75"/>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F76"/>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F77"/>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F78"/>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F79"/>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F80"/>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F81"/>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F82"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M4" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}"/>
@@ -8086,7 +8793,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I18:I1048576 L18:L1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="I83:I1048576 L83:L1048576" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -8094,10 +8801,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF1EAA0-8A30-4F1C-A86F-F04BCE344154}">
   <sheetPr codeName="Hoja2"/>
-  <dimension ref="A1:E1134"/>
+  <dimension ref="A1:E1147"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A1131" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1135" sqref="B1135:B1147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17207,6 +17914,110 @@
         <v>2280</v>
       </c>
     </row>
+    <row r="1135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1135" t="s">
+        <v>2296</v>
+      </c>
+      <c r="B1135" t="s">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1136" t="s">
+        <v>2297</v>
+      </c>
+      <c r="B1136" t="s">
+        <v>2310</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1137" t="s">
+        <v>2298</v>
+      </c>
+      <c r="B1137" t="s">
+        <v>2311</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1138" t="s">
+        <v>2299</v>
+      </c>
+      <c r="B1138" t="s">
+        <v>2312</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1139" t="s">
+        <v>2300</v>
+      </c>
+      <c r="B1139" t="s">
+        <v>2313</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1140" t="s">
+        <v>2301</v>
+      </c>
+      <c r="B1140" t="s">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1141" t="s">
+        <v>2302</v>
+      </c>
+      <c r="B1141" t="s">
+        <v>2315</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1142" t="s">
+        <v>2303</v>
+      </c>
+      <c r="B1142" t="s">
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1143" t="s">
+        <v>2304</v>
+      </c>
+      <c r="B1143" t="s">
+        <v>2317</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1144" t="s">
+        <v>2305</v>
+      </c>
+      <c r="B1144" t="s">
+        <v>2318</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1145" t="s">
+        <v>2306</v>
+      </c>
+      <c r="B1145" t="s">
+        <v>2319</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1146" t="s">
+        <v>2307</v>
+      </c>
+      <c r="B1146" t="s">
+        <v>2320</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1147" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1147" t="s">
+        <v>2321</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B1134" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B1119">

</xml_diff>

<commit_message>
Se mejoraron las esperas
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FE2B2D-8BB3-448D-8E34-20BBB7A0F6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44283A35-134F-4FFE-AE1A-4DDBFDD81795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-4020" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2394" uniqueCount="2325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2456" uniqueCount="2329">
   <si>
     <t>Hogar</t>
   </si>
@@ -6995,16 +6995,28 @@
     <t>2.4</t>
   </si>
   <si>
-    <t>05</t>
-  </si>
-  <si>
     <t>5.9</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>01 02</t>
+    <t>1.2 1.38 5.9</t>
+  </si>
+  <si>
+    <t>0 0 2</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5.11</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0320/01</t>
+  </si>
+  <si>
+    <t>8d231fd9-4685-464b-a9e1-7db18fcc137c</t>
   </si>
 </sst>
 </file>
@@ -7404,10 +7416,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7469,7 +7481,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>192</v>
+        <v>320</v>
       </c>
       <c r="C2" s="3">
         <v>45103</v>
@@ -7478,30 +7490,30 @@
         <v>2244</v>
       </c>
       <c r="E2" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2" si="0">CONCATENATE(TEXT(B2,"0000"),"/",TEXT(H2,"00"))</f>
-        <v>0192/01</v>
+        <v>0320/01</v>
       </c>
       <c r="G2" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F2),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>755f34f5-c8d7-4162-bbfa-10a6e7a5a7df</v>
+        <v>8d231fd9-4685-464b-a9e1-7db18fcc137c</v>
       </c>
       <c r="H2" s="5">
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>2323</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>2290</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>2321</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>2289</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>2290</v>
@@ -7512,10 +7524,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>238</v>
+        <v>70</v>
       </c>
       <c r="C3" s="3">
-        <v>45093</v>
+        <v>45107</v>
       </c>
       <c r="D3" t="s">
         <v>2244</v>
@@ -7524,27 +7536,27 @@
         <v>2245</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3" si="1">CONCATENATE(TEXT(B3,"0000"),"/",TEXT(H3,"00"))</f>
-        <v>0238/01</v>
+        <f t="shared" ref="F3:F19" si="1">CONCATENATE(TEXT(B3,"0000"),"/",TEXT(H3,"00"))</f>
+        <v>0070/02</v>
       </c>
       <c r="G3" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F3),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>5fd5ccdc-af65-4180-9562-3ff6b3407370</v>
+        <v>e069d11c-5e65-4ba3-ba65-8bc1adce2860</v>
       </c>
       <c r="H3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>2290</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>2292</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>2289</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>2290</v>
@@ -7555,10 +7567,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>16</v>
+        <v>283</v>
       </c>
       <c r="C4" s="3">
-        <v>45104</v>
+        <v>45107</v>
       </c>
       <c r="D4" t="s">
         <v>2244</v>
@@ -7567,30 +7579,30 @@
         <v>2245</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F13" si="2">CONCATENATE(TEXT(B4,"0000"),"/",TEXT(H4,"00"))</f>
-        <v>0016/01</v>
+        <f t="shared" si="1"/>
+        <v>0283/01</v>
       </c>
       <c r="G4" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F4),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
+        <v>f8c71a6e-498f-40e4-a971-865a2bad5eb4</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>2319</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>2320</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0</v>
+      <c r="M4" s="2" t="s">
+        <v>2290</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -7598,39 +7610,39 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>301</v>
+        <v>203</v>
       </c>
       <c r="C5" s="3">
-        <v>45098</v>
+        <v>45107</v>
       </c>
       <c r="D5" t="s">
         <v>2244</v>
       </c>
       <c r="E5" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ref="F5:F10" si="3">CONCATENATE(TEXT(B5,"0000"),"/",TEXT(H5,"00"))</f>
-        <v>0301/01</v>
+        <f t="shared" si="1"/>
+        <v>0203/01</v>
       </c>
       <c r="G5" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F5),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>1ab440ce-f136-4a23-99b4-693c02499e9d</v>
+        <v>e94f1520-8ef4-4511-a8ec-5083b848431c</v>
       </c>
       <c r="H5" s="5">
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>2290</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>2324</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>2289</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>2290</v>
@@ -7641,39 +7653,39 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C6" s="3">
-        <v>45092</v>
+        <v>45107</v>
       </c>
       <c r="D6" t="s">
         <v>2244</v>
       </c>
       <c r="E6" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="3"/>
-        <v>0298/01</v>
+        <f t="shared" si="1"/>
+        <v>0295/01</v>
       </c>
       <c r="G6" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F6),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>93a5aba7-7493-4eac-bd7a-55f3ba79ca45</v>
+        <v>7d824e1d-9db7-4658-a783-9fab5f93fffc</v>
       </c>
       <c r="H6" s="5">
         <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>2290</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>2292</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>2289</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>2290</v>
@@ -7684,10 +7696,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>30</v>
+        <v>171</v>
       </c>
       <c r="C7" s="3">
-        <v>45099</v>
+        <v>45107</v>
       </c>
       <c r="D7" t="s">
         <v>2244</v>
@@ -7696,30 +7708,30 @@
         <v>2245</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="3"/>
-        <v>0030/02</v>
+        <f t="shared" si="1"/>
+        <v>0171/01</v>
       </c>
       <c r="G7" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F7),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>22004b81-0e55-4f9c-a90d-8c4031e1ace8</v>
+        <v>5007e9af-6262-423e-98e1-0fc49750d756</v>
       </c>
       <c r="H7" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>2319</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>2289</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0</v>
+      <c r="M7" s="2" t="s">
+        <v>2290</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -7727,39 +7739,39 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>303</v>
+        <v>106</v>
       </c>
       <c r="C8" s="3">
-        <v>45097</v>
+        <v>45107</v>
       </c>
       <c r="D8" t="s">
         <v>2244</v>
       </c>
       <c r="E8" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="3"/>
-        <v>0303/01</v>
+        <f t="shared" si="1"/>
+        <v>0106/02</v>
       </c>
       <c r="G8" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F8),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>6e2d5351-3cb7-4c98-90d7-79789b29d936</v>
+        <v>77c51c15-e6a1-4fef-b5bd-9bb349469be4</v>
       </c>
       <c r="H8" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>2290</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>2292</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>2289</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>2290</v>
@@ -7770,10 +7782,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>296</v>
+        <v>210</v>
       </c>
       <c r="C9" s="3">
-        <v>45099</v>
+        <v>45107</v>
       </c>
       <c r="D9" t="s">
         <v>2244</v>
@@ -7782,27 +7794,27 @@
         <v>2245</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="3"/>
-        <v>0296/01</v>
+        <f t="shared" si="1"/>
+        <v>0210/01</v>
       </c>
       <c r="G9" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F9),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>519bb9e8-7948-451a-a8dd-2b92d420ae7f</v>
+        <v>99e4457f-dc39-440d-9b81-7a19994aff4f</v>
       </c>
       <c r="H9" s="5">
         <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>2290</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>2292</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>2289</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>2290</v>
@@ -7813,42 +7825,42 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>177</v>
+        <v>253</v>
       </c>
       <c r="C10" s="3">
-        <v>45099</v>
+        <v>45107</v>
       </c>
       <c r="D10" t="s">
         <v>2244</v>
       </c>
       <c r="E10" t="s">
-        <v>2250</v>
+        <v>2245</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="3"/>
-        <v>0177/01</v>
+        <f t="shared" si="1"/>
+        <v>0253/01</v>
       </c>
       <c r="G10" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F10),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>7afe12e5-7259-4b81-b39c-d5872d19907a</v>
+        <v>6d30fed4-850e-4080-8a82-89ff042e1419</v>
       </c>
       <c r="H10" s="5">
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>2322</v>
+        <v>2326</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>2323</v>
+        <v>2325</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>2292</v>
+        <v>2290</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>2289</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0</v>
+        <v>2290</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>2290</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -7856,10 +7868,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1">
-        <v>16</v>
+        <v>148</v>
       </c>
       <c r="C11" s="3">
-        <v>45105</v>
+        <v>45107</v>
       </c>
       <c r="D11" t="s">
         <v>2244</v>
@@ -7868,30 +7880,30 @@
         <v>2245</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="2"/>
-        <v>0016/01</v>
+        <f t="shared" si="1"/>
+        <v>0148/01</v>
       </c>
       <c r="G11" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F11),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
+        <v>544b8ff7-f2df-4584-8c9d-fe746daea693</v>
       </c>
       <c r="H11" s="5">
         <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>2319</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>2320</v>
-      </c>
-      <c r="M11" s="2">
-        <v>0</v>
+      <c r="M11" s="2" t="s">
+        <v>2290</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -7899,10 +7911,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>16</v>
+        <v>234</v>
       </c>
       <c r="C12" s="3">
-        <v>45106</v>
+        <v>45107</v>
       </c>
       <c r="D12" t="s">
         <v>2244</v>
@@ -7911,30 +7923,30 @@
         <v>2245</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="2"/>
-        <v>0016/01</v>
+        <f t="shared" si="1"/>
+        <v>0234/01</v>
       </c>
       <c r="G12" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F12),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
+        <v>61473b6d-0f2c-4a8e-a8f3-eaffe88cee60</v>
       </c>
       <c r="H12" s="5">
         <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>2319</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>2320</v>
-      </c>
-      <c r="M12" s="2">
-        <v>0</v>
+      <c r="M12" s="2" t="s">
+        <v>2290</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -7942,7 +7954,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C13" s="3">
         <v>45107</v>
@@ -7954,87 +7966,407 @@
         <v>2245</v>
       </c>
       <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>0040/01</v>
+      </c>
+      <c r="G13" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F13),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>2dfcd22d-1e57-48ae-ab25-338f0960370e</v>
+      </c>
+      <c r="H13" s="5">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>2290</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>2290</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>300</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45107</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>0300/01</v>
+      </c>
+      <c r="G14" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F14),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>8479d197-d10b-4aec-8284-e72962bc7719</v>
+      </c>
+      <c r="H14" s="5">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>2290</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>2290</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>265</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45107</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>0265/02</v>
+      </c>
+      <c r="G15" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F15),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>2bd6129c-7a32-4378-bdc1-0081eebbb548</v>
+      </c>
+      <c r="H15" s="5">
+        <v>2</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>2290</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>2290</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>65</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45107</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>0065/01</v>
+      </c>
+      <c r="G16" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F16),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>8f7f3866-2286-4238-9a04-fa0c5401c2c4</v>
+      </c>
+      <c r="H16" s="5">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>2290</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>2290</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>283</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45104</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>0283/01</v>
+      </c>
+      <c r="G17" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F17),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>f8c71a6e-498f-40e4-a971-865a2bad5eb4</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>2290</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>2290</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>2292</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>228</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45104</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>0228/01</v>
+      </c>
+      <c r="G18" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F18),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>bbfd3757-166f-4a75-a998-9c0ca6b58ef4</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>2290</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>2290</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>2292</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>254</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45104</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v>0254/01</v>
+      </c>
+      <c r="G19" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F19),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>89534233-c46a-498f-8704-fffda132b9b8</v>
+      </c>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>2321</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>2322</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>2292</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>2290</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>16</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45106</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" ref="F20:F21" si="2">CONCATENATE(TEXT(B20,"0000"),"/",TEXT(H20,"00"))</f>
+        <v>0016/01</v>
+      </c>
+      <c r="G20" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F20),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>2319</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>2320</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>16</v>
+      </c>
+      <c r="C21" s="3">
+        <v>45107</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2244</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F21" t="str">
         <f t="shared" si="2"/>
         <v>0016/01</v>
       </c>
-      <c r="G13" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F13),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+      <c r="G21" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F21),Sheet1!$A$1:$B$1251,2,FALSE)</f>
         <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H21" s="5">
         <v>1</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="K13" s="2" t="s">
+      <c r="I21" s="2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>2319</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>2320</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M21" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F14"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F15"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F16"/>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18"/>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20"/>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F22"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F23"/>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F24"/>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F25"/>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F26"/>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F27"/>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F28"/>
     </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F29"/>
     </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F30"/>
     </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F31"/>
     </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F32"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">
@@ -8136,10 +8468,34 @@
     <row r="65" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F65"/>
     </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F66"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F67"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F68"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F71"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F72"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F73"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C4:C13">
-    <sortCondition ref="C4:C13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C20:C21">
+    <sortCondition ref="C20:C21"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
@@ -8149,7 +8505,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I66:I1048576 L66:L1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="I74:I1048576 L74:L1048576" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -8157,10 +8513,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF1EAA0-8A30-4F1C-A86F-F04BCE344154}">
   <sheetPr codeName="Hoja2"/>
-  <dimension ref="A1:E1147"/>
+  <dimension ref="A1:E1148"/>
   <sheetViews>
     <sheetView topLeftCell="A1131" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1135" sqref="B1135:B1147"/>
+      <selection activeCell="B1148" sqref="B1148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17374,12 +17730,21 @@
         <v>2318</v>
       </c>
     </row>
+    <row r="1148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1148" t="s">
+        <v>2327</v>
+      </c>
+      <c r="B1148" t="s">
+        <v>2328</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B1134" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B1119">
       <sortCondition ref="A1:A1119"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Integracion de bases de datos
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44283A35-134F-4FFE-AE1A-4DDBFDD81795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92875B95-2D35-482A-8CCD-4A21DB60C378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
+    <workbookView xWindow="-20610" yWindow="-4020" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2456" uniqueCount="2329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="2326">
   <si>
     <t>Hogar</t>
   </si>
@@ -6899,9 +6899,6 @@
     <t>Cuando un servicio esté vacío o si un servicio no lleva donante, se debe colocar '0'</t>
   </si>
   <si>
-    <t>1.9</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -6989,44 +6986,37 @@
     <t>b572048a-fde5-4882-8b63-c82cd596227c</t>
   </si>
   <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>2.4</t>
-  </si>
-  <si>
-    <t>5.9</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>1.2 1.38 5.9</t>
   </si>
   <si>
     <t>0 0 2</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>5.11</t>
-  </si>
-  <si>
     <t>PU/GRE/CG/0320/01</t>
   </si>
   <si>
     <t>8d231fd9-4685-464b-a9e1-7db18fcc137c</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0322/01</t>
+  </si>
+  <si>
+    <t>5ea2fd3c-9508-4b30-a45b-c0ae2b39ed1f</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0321/01</t>
+  </si>
+  <si>
+    <t>f4ec394d-91e8-4696-b9d2-d0fb09ad0fa7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;PU/GRE/CG/&quot;0000"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -7070,13 +7060,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -7416,10 +7405,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:M73"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7430,7 +7419,7 @@
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="38.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="5"/>
+    <col min="8" max="8" width="11.42578125" style="2"/>
     <col min="9" max="10" width="11.42578125" style="2" customWidth="1"/>
     <col min="11" max="13" width="11.42578125" style="2"/>
   </cols>
@@ -7457,7 +7446,7 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="2" t="s">
         <v>2243</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -7470,7 +7459,7 @@
         <v>2285</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>2286</v>
@@ -7481,10 +7470,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C2" s="3">
-        <v>45103</v>
+        <v>45115</v>
       </c>
       <c r="D2" t="s">
         <v>2244</v>
@@ -7494,29 +7483,29 @@
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2" si="0">CONCATENATE(TEXT(B2,"0000"),"/",TEXT(H2,"00"))</f>
-        <v>0320/01</v>
+        <v>0321/01</v>
       </c>
       <c r="G2" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F2),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>8d231fd9-4685-464b-a9e1-7db18fcc137c</v>
-      </c>
-      <c r="H2" s="5">
-        <v>1</v>
+        <v>f4ec394d-91e8-4696-b9d2-d0fb09ad0fa7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>2291</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>2323</v>
+        <v>2318</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>2324</v>
+        <v>2319</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -7524,10 +7513,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>70</v>
+        <v>322</v>
       </c>
       <c r="C3" s="3">
-        <v>45107</v>
+        <v>45116</v>
       </c>
       <c r="D3" t="s">
         <v>2244</v>
@@ -7536,837 +7525,117 @@
         <v>2245</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F19" si="1">CONCATENATE(TEXT(B3,"0000"),"/",TEXT(H3,"00"))</f>
-        <v>0070/02</v>
+        <f t="shared" ref="F3" si="1">CONCATENATE(TEXT(B3,"0000"),"/",TEXT(H3,"00"))</f>
+        <v>0322/01</v>
       </c>
       <c r="G3" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F3),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>e069d11c-5e65-4ba3-ba65-8bc1adce2860</v>
-      </c>
-      <c r="H3" s="5">
-        <v>2</v>
+        <v>5ea2fd3c-9508-4b30-a45b-c0ae2b39ed1f</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>2291</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>2326</v>
+        <v>2318</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>2325</v>
+        <v>2319</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>283</v>
-      </c>
-      <c r="C4" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" si="1"/>
-        <v>0283/01</v>
-      </c>
-      <c r="G4" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F4),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>f8c71a6e-498f-40e4-a971-865a2bad5eb4</v>
-      </c>
-      <c r="H4" s="5">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>2290</v>
-      </c>
+      <c r="F4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>203</v>
-      </c>
-      <c r="C5" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="1"/>
-        <v>0203/01</v>
-      </c>
-      <c r="G5" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F5),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>e94f1520-8ef4-4511-a8ec-5083b848431c</v>
-      </c>
-      <c r="H5" s="5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>2290</v>
-      </c>
+      <c r="F5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>295</v>
-      </c>
-      <c r="C6" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="1"/>
-        <v>0295/01</v>
-      </c>
-      <c r="G6" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F6),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>7d824e1d-9db7-4658-a783-9fab5f93fffc</v>
-      </c>
-      <c r="H6" s="5">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>2290</v>
-      </c>
+      <c r="F6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>171</v>
-      </c>
-      <c r="C7" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="1"/>
-        <v>0171/01</v>
-      </c>
-      <c r="G7" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F7),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>5007e9af-6262-423e-98e1-0fc49750d756</v>
-      </c>
-      <c r="H7" s="5">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>2290</v>
-      </c>
+      <c r="F7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>106</v>
-      </c>
-      <c r="C8" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="1"/>
-        <v>0106/02</v>
-      </c>
-      <c r="G8" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F8),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>77c51c15-e6a1-4fef-b5bd-9bb349469be4</v>
-      </c>
-      <c r="H8" s="5">
-        <v>2</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>2290</v>
-      </c>
+      <c r="F8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>210</v>
-      </c>
-      <c r="C9" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="1"/>
-        <v>0210/01</v>
-      </c>
-      <c r="G9" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F9),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>99e4457f-dc39-440d-9b81-7a19994aff4f</v>
-      </c>
-      <c r="H9" s="5">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>2290</v>
-      </c>
+      <c r="F9"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1">
-        <v>253</v>
-      </c>
-      <c r="C10" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="1"/>
-        <v>0253/01</v>
-      </c>
-      <c r="G10" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F10),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>6d30fed4-850e-4080-8a82-89ff042e1419</v>
-      </c>
-      <c r="H10" s="5">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>2290</v>
-      </c>
+      <c r="F10"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1">
-        <v>148</v>
-      </c>
-      <c r="C11" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="1"/>
-        <v>0148/01</v>
-      </c>
-      <c r="G11" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F11),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>544b8ff7-f2df-4584-8c9d-fe746daea693</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>2290</v>
-      </c>
+      <c r="F11"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
-        <v>234</v>
-      </c>
-      <c r="C12" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="1"/>
-        <v>0234/01</v>
-      </c>
-      <c r="G12" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F12),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>61473b6d-0f2c-4a8e-a8f3-eaffe88cee60</v>
-      </c>
-      <c r="H12" s="5">
-        <v>1</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>2290</v>
-      </c>
+      <c r="F12"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1">
-        <v>40</v>
-      </c>
-      <c r="C13" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="1"/>
-        <v>0040/01</v>
-      </c>
-      <c r="G13" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F13),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>2dfcd22d-1e57-48ae-ab25-338f0960370e</v>
-      </c>
-      <c r="H13" s="5">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>2290</v>
-      </c>
+      <c r="F13"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1">
-        <v>300</v>
-      </c>
-      <c r="C14" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E14" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="1"/>
-        <v>0300/01</v>
-      </c>
-      <c r="G14" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F14),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>8479d197-d10b-4aec-8284-e72962bc7719</v>
-      </c>
-      <c r="H14" s="5">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>2290</v>
-      </c>
+      <c r="F14"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1">
-        <v>265</v>
-      </c>
-      <c r="C15" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E15" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="1"/>
-        <v>0265/02</v>
-      </c>
-      <c r="G15" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F15),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>2bd6129c-7a32-4378-bdc1-0081eebbb548</v>
-      </c>
-      <c r="H15" s="5">
-        <v>2</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>2290</v>
-      </c>
+      <c r="F15"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1">
-        <v>65</v>
-      </c>
-      <c r="C16" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D16" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="1"/>
-        <v>0065/01</v>
-      </c>
-      <c r="G16" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F16),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>8f7f3866-2286-4238-9a04-fa0c5401c2c4</v>
-      </c>
-      <c r="H16" s="5">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>2290</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1">
-        <v>283</v>
-      </c>
-      <c r="C17" s="3">
-        <v>45104</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E17" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="1"/>
-        <v>0283/01</v>
-      </c>
-      <c r="G17" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F17),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>f8c71a6e-498f-40e4-a971-865a2bad5eb4</v>
-      </c>
-      <c r="H17" s="5">
-        <v>1</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>2292</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>2289</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>2290</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1">
-        <v>228</v>
-      </c>
-      <c r="C18" s="3">
-        <v>45104</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E18" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="1"/>
-        <v>0228/01</v>
-      </c>
-      <c r="G18" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F18),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>bbfd3757-166f-4a75-a998-9c0ca6b58ef4</v>
-      </c>
-      <c r="H18" s="5">
-        <v>1</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>2290</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>2292</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>2289</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>2290</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1">
-        <v>254</v>
-      </c>
-      <c r="C19" s="3">
-        <v>45104</v>
-      </c>
-      <c r="D19" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E19" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F19" t="str">
-        <f t="shared" si="1"/>
-        <v>0254/01</v>
-      </c>
-      <c r="G19" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F19),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>89534233-c46a-498f-8704-fffda132b9b8</v>
-      </c>
-      <c r="H19" s="5">
-        <v>1</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>2321</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>2322</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>2292</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>2289</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>2290</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1">
-        <v>16</v>
-      </c>
-      <c r="C20" s="3">
-        <v>45106</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E20" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" ref="F20:F21" si="2">CONCATENATE(TEXT(B20,"0000"),"/",TEXT(H20,"00"))</f>
-        <v>0016/01</v>
-      </c>
-      <c r="G20" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F20),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
-      </c>
-      <c r="H20" s="5">
-        <v>1</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>2319</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>2320</v>
-      </c>
-      <c r="M20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1">
-        <v>16</v>
-      </c>
-      <c r="C21" s="3">
-        <v>45107</v>
-      </c>
-      <c r="D21" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E21" t="s">
-        <v>2245</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" si="2"/>
-        <v>0016/01</v>
-      </c>
-      <c r="G21" t="str">
-        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F21),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>26e19b20-4b58-415f-8870-3a8e97b31b62</v>
-      </c>
-      <c r="H21" s="5">
-        <v>1</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>2326</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>2325</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>2319</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>2320</v>
-      </c>
-      <c r="M21" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F32"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">
@@ -8435,68 +7704,8 @@
     <row r="54" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F54"/>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F55"/>
-    </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F56"/>
-    </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F57"/>
-    </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F58"/>
-    </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F59"/>
-    </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F60"/>
-    </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F61"/>
-    </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F62"/>
-    </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F63"/>
-    </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F64"/>
-    </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F65"/>
-    </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F66"/>
-    </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F67"/>
-    </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F68"/>
-    </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F69"/>
-    </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F70"/>
-    </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F71"/>
-    </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F72"/>
-    </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F73"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C20:C21">
-    <sortCondition ref="C20:C21"/>
-  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
@@ -8505,7 +7714,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I74:I1048576 L74:L1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="I55:I1048576 L55:L1048576" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -8513,17 +7722,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF1EAA0-8A30-4F1C-A86F-F04BCE344154}">
   <sheetPr codeName="Hoja2"/>
-  <dimension ref="A1:E1148"/>
+  <dimension ref="A1:E1150"/>
   <sheetViews>
     <sheetView topLeftCell="A1131" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1148" sqref="B1148"/>
+      <selection activeCell="A1149" sqref="A1149:B1150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="5" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8542,7 +7751,7 @@
       <c r="B2" t="s">
         <v>595</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>2246</v>
       </c>
       <c r="E2" t="s">
@@ -8586,7 +7795,7 @@
       <c r="B6" t="s">
         <v>1611</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>2249</v>
       </c>
       <c r="E6" t="s">
@@ -8619,7 +7828,7 @@
       <c r="B9" t="s">
         <v>557</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>2287</v>
       </c>
       <c r="E9" t="s">
@@ -17628,114 +16837,130 @@
     </row>
     <row r="1135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1135" t="s">
-        <v>2293</v>
+        <v>2292</v>
       </c>
       <c r="B1135" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="1136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1136" t="s">
-        <v>2294</v>
+        <v>2293</v>
       </c>
       <c r="B1136" t="s">
-        <v>2307</v>
+        <v>2306</v>
       </c>
     </row>
     <row r="1137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1137" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="B1137" t="s">
-        <v>2308</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="1138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1138" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="B1138" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="1139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1139" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
       <c r="B1139" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="1140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1140" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
       <c r="B1140" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="1141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1141" t="s">
-        <v>2299</v>
+        <v>2298</v>
       </c>
       <c r="B1141" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="1142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1142" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="B1142" t="s">
-        <v>2313</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="1143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1143" t="s">
-        <v>2301</v>
+        <v>2300</v>
       </c>
       <c r="B1143" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="1144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1144" t="s">
-        <v>2302</v>
+        <v>2301</v>
       </c>
       <c r="B1144" t="s">
-        <v>2315</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="1145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1145" t="s">
-        <v>2303</v>
+        <v>2302</v>
       </c>
       <c r="B1145" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="1146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1146" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
       <c r="B1146" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="1147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1147" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
       <c r="B1147" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="1148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1148" t="s">
-        <v>2327</v>
+        <v>2320</v>
       </c>
       <c r="B1148" t="s">
-        <v>2328</v>
+        <v>2321</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1149" t="s">
+        <v>2322</v>
+      </c>
+      <c r="B1149" t="s">
+        <v>2323</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1150" t="s">
+        <v>2324</v>
+      </c>
+      <c r="B1150" t="s">
+        <v>2325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se integra la bd para almacenar los servicios
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -8,29 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92875B95-2D35-482A-8CCD-4A21DB60C378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DEDDC0-BEFD-4B50-A286-B384F653809D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-4020" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="fk" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$B$1134</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="2326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="2331">
   <si>
     <t>Hogar</t>
   </si>
@@ -6986,12 +6996,6 @@
     <t>b572048a-fde5-4882-8b63-c82cd596227c</t>
   </si>
   <si>
-    <t>1.2 1.38 5.9</t>
-  </si>
-  <si>
-    <t>0 0 2</t>
-  </si>
-  <si>
     <t>PU/GRE/CG/0320/01</t>
   </si>
   <si>
@@ -7008,6 +7012,27 @@
   </si>
   <si>
     <t>f4ec394d-91e8-4696-b9d2-d0fb09ad0fa7</t>
+  </si>
+  <si>
+    <t>1.2 1.38</t>
+  </si>
+  <si>
+    <t>0 0</t>
+  </si>
+  <si>
+    <t>lugar</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>motivo</t>
+  </si>
+  <si>
+    <t>Monitoreo</t>
+  </si>
+  <si>
+    <t>02</t>
   </si>
 </sst>
 </file>
@@ -7405,23 +7430,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="38.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="2"/>
-    <col min="9" max="10" width="11.42578125" style="2" customWidth="1"/>
-    <col min="11" max="13" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -7470,33 +7497,33 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>321</v>
+        <v>162</v>
       </c>
       <c r="C2" s="3">
-        <v>45115</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2245</v>
+        <v>45113</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2" si="0">CONCATENATE(TEXT(B2,"0000"),"/",TEXT(H2,"00"))</f>
-        <v>0321/01</v>
+        <v>0162/02</v>
       </c>
       <c r="G2" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F2),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>f4ec394d-91e8-4696-b9d2-d0fb09ad0fa7</v>
+        <v>00b3c431-dec9-47e6-a3d9-982775f6cc93</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>2291</v>
+        <v>2330</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>2318</v>
+        <v>2324</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>2319</v>
+        <v>2325</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>2289</v>
@@ -7513,33 +7540,33 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>322</v>
+        <v>154</v>
       </c>
       <c r="C3" s="3">
-        <v>45116</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2244</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2245</v>
+        <v>45112</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3" si="1">CONCATENATE(TEXT(B3,"0000"),"/",TEXT(H3,"00"))</f>
-        <v>0322/01</v>
+        <f t="shared" ref="F3:F5" si="1">CONCATENATE(TEXT(B3,"0000"),"/",TEXT(H3,"00"))</f>
+        <v>0154/01</v>
       </c>
       <c r="G3" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F3),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>5ea2fd3c-9508-4b30-a45b-c0ae2b39ed1f</v>
+        <v>393c3265-346e-4910-a569-8e90a9fbe8b0</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>2291</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>2318</v>
+        <v>2324</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>2319</v>
+        <v>2325</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>2289</v>
@@ -7552,157 +7579,90 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F4"/>
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>142</v>
+      </c>
+      <c r="C4" s="3">
+        <v>45112</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="1"/>
+        <v>0142/01</v>
+      </c>
+      <c r="G4" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F4),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>8ffab94f-63f3-48d0-874f-9087bd553bcf</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>2289</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F14"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F15"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F16"/>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18"/>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20"/>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23"/>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24"/>
-    </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25"/>
-    </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F26"/>
-    </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F27"/>
-    </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F28"/>
-    </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F29"/>
-    </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F30"/>
-    </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F31"/>
-    </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F32"/>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33"/>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F34"/>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F35"/>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F36"/>
-    </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F37"/>
-    </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F38"/>
-    </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F39"/>
-    </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F40"/>
-    </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F41"/>
-    </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F42"/>
-    </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F43"/>
-    </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F44"/>
-    </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F45"/>
-    </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F46"/>
-    </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F47"/>
-    </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F48"/>
-    </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F49"/>
-    </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F51"/>
-    </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F52"/>
-    </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F53"/>
-    </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F54"/>
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45111</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>0020/01</v>
+      </c>
+      <c r="G5" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F5),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>d10697ff-c6d4-47a0-b99e-d05d8bd07044</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>2289</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}"/>
@@ -7714,7 +7674,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I55:I1048576 L55:L1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="I6:I1048576 L6:L1048576" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -7724,7 +7684,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:E1150"/>
   <sheetViews>
-    <sheetView topLeftCell="A1131" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A1119" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1149" sqref="A1149:B1150"/>
     </sheetView>
   </sheetViews>
@@ -16941,26 +16901,26 @@
     </row>
     <row r="1148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1148" t="s">
-        <v>2320</v>
+        <v>2318</v>
       </c>
       <c r="B1148" t="s">
-        <v>2321</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="1149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1149" t="s">
-        <v>2322</v>
+        <v>2320</v>
       </c>
       <c r="B1149" t="s">
-        <v>2323</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="1150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1150" t="s">
-        <v>2324</v>
+        <v>2322</v>
       </c>
       <c r="B1150" t="s">
-        <v>2325</v>
+        <v>2323</v>
       </c>
     </row>
   </sheetData>
@@ -16972,4 +16932,69 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A7FDDB-97D5-4BD7-B377-27BE6F6D7533}">
+  <dimension ref="A2:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2327</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2326</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2327</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2250</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2245</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2329</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega el formulario 01 y las clases del hogar
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DEDDC0-BEFD-4B50-A286-B384F653809D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7613C9-AFDD-43C9-8ED3-C0799282B5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
+    <workbookView xWindow="-20610" yWindow="-4020" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="2331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2441" uniqueCount="2342">
   <si>
     <t>Hogar</t>
   </si>
@@ -7014,12 +7014,6 @@
     <t>f4ec394d-91e8-4696-b9d2-d0fb09ad0fa7</t>
   </si>
   <si>
-    <t>1.2 1.38</t>
-  </si>
-  <si>
-    <t>0 0</t>
-  </si>
-  <si>
     <t>lugar</t>
   </si>
   <si>
@@ -7032,7 +7026,46 @@
     <t>Monitoreo</t>
   </si>
   <si>
+    <t>b9ad52fa-d4ec-454d-b55e-9dbd1e3f5561</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0323/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0349/01</t>
+  </si>
+  <si>
+    <t>bf850588-6b9c-44f9-bd58-f1934285a06e</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0350/01</t>
+  </si>
+  <si>
+    <t>PU/GRE/CG/0350/02</t>
+  </si>
+  <si>
+    <t>2c24e14c-2e4c-40b9-a49d-acd6dd9d2bb1</t>
+  </si>
+  <si>
+    <t>695c4093-bc6b-42ce-a5bc-c4923c4ca491</t>
+  </si>
+  <si>
     <t>02</t>
+  </si>
+  <si>
+    <t>1.2 1.38 5.9</t>
+  </si>
+  <si>
+    <t>0 0 2</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>03</t>
   </si>
 </sst>
 </file>
@@ -7430,23 +7463,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2DBA90-5F51-4CD3-860D-DE113D48D65A}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="38.28515625" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="2" customWidth="1"/>
     <col min="11" max="11" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="11.42578125" style="2"/>
   </cols>
@@ -7497,39 +7530,39 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>162</v>
+        <v>310</v>
       </c>
       <c r="C2" s="3">
-        <v>45113</v>
+        <v>45134</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2" si="0">CONCATENATE(TEXT(B2,"0000"),"/",TEXT(H2,"00"))</f>
-        <v>0162/02</v>
+        <v>0310/01</v>
       </c>
       <c r="G2" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F2),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>00b3c431-dec9-47e6-a3d9-982775f6cc93</v>
+        <v>11e39041-f9fd-45b6-94b8-c301b9910979</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>2330</v>
+        <v>2291</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>2324</v>
+        <v>2289</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>2325</v>
+        <v>2289</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>2289</v>
+        <v>2291</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>2289</v>
+        <v>2339</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>2289</v>
@@ -7540,39 +7573,39 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>154</v>
+        <v>31</v>
       </c>
       <c r="C3" s="3">
-        <v>45112</v>
+        <v>45135</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F5" si="1">CONCATENATE(TEXT(B3,"0000"),"/",TEXT(H3,"00"))</f>
-        <v>0154/01</v>
+        <f t="shared" ref="F3:F8" si="1">CONCATENATE(TEXT(B3,"0000"),"/",TEXT(H3,"00"))</f>
+        <v>0031/01</v>
       </c>
       <c r="G3" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F3),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>393c3265-346e-4910-a569-8e90a9fbe8b0</v>
+        <v>899f6639-2fee-49e4-adbd-9ac1c7d4478f</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>2291</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>2324</v>
+        <v>2289</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>2325</v>
+        <v>2289</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>2289</v>
+        <v>2291</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>2289</v>
+        <v>2339</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>2289</v>
@@ -7583,39 +7616,39 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>142</v>
+        <v>310</v>
       </c>
       <c r="C4" s="3">
-        <v>45112</v>
+        <v>45132</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
-        <v>0142/01</v>
+        <v>0310/01</v>
       </c>
       <c r="G4" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F4),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>8ffab94f-63f3-48d0-874f-9087bd553bcf</v>
+        <v>11e39041-f9fd-45b6-94b8-c301b9910979</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>2291</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>2324</v>
+        <v>2289</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>2325</v>
+        <v>2289</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>2289</v>
+        <v>2336</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>2289</v>
+        <v>2339</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>2289</v>
@@ -7626,33 +7659,33 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>20</v>
+        <v>289</v>
       </c>
       <c r="C5" s="3">
-        <v>45111</v>
+        <v>45135</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
-        <v>0020/01</v>
+        <v>0289/01</v>
       </c>
       <c r="G5" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F5),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>d10697ff-c6d4-47a0-b99e-d05d8bd07044</v>
+        <v>b3174ba3-e2b1-4f80-bf0b-d5bfefd91310</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>2291</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>2324</v>
+        <v>2337</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>2325</v>
+        <v>2338</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>2289</v>
@@ -7661,6 +7694,565 @@
         <v>2289</v>
       </c>
       <c r="M5" s="2" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>219</v>
+      </c>
+      <c r="C6" s="3">
+        <v>45135</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>0219/01</v>
+      </c>
+      <c r="G6" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F6),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>f75cda6e-9fff-49e0-b451-f1a96abcecc8</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>285</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45136</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>0285/01</v>
+      </c>
+      <c r="G7" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F7),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>86edd196-f574-4477-a266-527620fa546a</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>49</v>
+      </c>
+      <c r="C8" s="3">
+        <v>45135</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>0049/05</v>
+      </c>
+      <c r="G8" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F8),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>f1774a4b-b951-4693-8757-467334b011d9</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>2340</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>288</v>
+      </c>
+      <c r="C9" s="3">
+        <v>45134</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" ref="F9:F15" si="2">CONCATENATE(TEXT(B9,"0000"),"/",TEXT(H9,"00"))</f>
+        <v>0288/01</v>
+      </c>
+      <c r="G9" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F9),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>8d61f76a-54b3-49fb-8bf4-760705670b34</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>90</v>
+      </c>
+      <c r="C10" s="3">
+        <v>45135</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="2"/>
+        <v>0090/02</v>
+      </c>
+      <c r="G10" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F10),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>f389fdf6-5f88-437a-a4a4-0ae1f5c736f5</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>2336</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>283</v>
+      </c>
+      <c r="C11" s="3">
+        <v>45135</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="2"/>
+        <v>0283/01</v>
+      </c>
+      <c r="G11" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F11),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>f8c71a6e-498f-40e4-a971-865a2bad5eb4</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>253</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45135</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="2"/>
+        <v>0253/01</v>
+      </c>
+      <c r="G12" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F12),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>6d30fed4-850e-4080-8a82-89ff042e1419</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>240</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45136</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="2"/>
+        <v>0240/01</v>
+      </c>
+      <c r="G13" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F13),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>bfb879e2-a577-4b7a-a781-0dabf1a4c387</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>203</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45136</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="2"/>
+        <v>0203/01</v>
+      </c>
+      <c r="G14" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F14),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>e94f1520-8ef4-4511-a8ec-5083b848431c</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>295</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45136</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="2"/>
+        <v>0295/01</v>
+      </c>
+      <c r="G15" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F15),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>7d824e1d-9db7-4658-a783-9fab5f93fffc</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>96</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45135</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" ref="F16:F18" si="3">CONCATENATE(TEXT(B16,"0000"),"/",TEXT(H16,"00"))</f>
+        <v>0096/01</v>
+      </c>
+      <c r="G16" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F16),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>b08752d8-7d73-47ee-9f2f-c182a6311b8f</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>263</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45136</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="3"/>
+        <v>0263/01</v>
+      </c>
+      <c r="G17" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F17),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>3a711287-08cc-42e5-9699-ce108b4b7d25</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>2291</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45136</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="3"/>
+        <v>0011/03</v>
+      </c>
+      <c r="G18" t="str">
+        <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F18),Sheet1!$A$1:$B$1251,2,FALSE)</f>
+        <v>d92e77e1-e7fc-4b11-a712-a8f4d651a79d</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>2341</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>2289</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>2289</v>
       </c>
     </row>
@@ -7674,7 +8266,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="I6:I1048576 L6:L1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="I19:I1048576 L19:L1048576" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -7682,10 +8274,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF1EAA0-8A30-4F1C-A86F-F04BCE344154}">
   <sheetPr codeName="Hoja2"/>
-  <dimension ref="A1:E1150"/>
+  <dimension ref="A1:E1154"/>
   <sheetViews>
-    <sheetView topLeftCell="A1119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1149" sqref="A1149:B1150"/>
+    <sheetView topLeftCell="A1143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1150" sqref="F1150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16921,6 +17513,38 @@
       </c>
       <c r="B1150" t="s">
         <v>2323</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1151" t="s">
+        <v>2329</v>
+      </c>
+      <c r="B1151" t="s">
+        <v>2328</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1152" t="s">
+        <v>2330</v>
+      </c>
+      <c r="B1152" t="s">
+        <v>2331</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1153" t="s">
+        <v>2332</v>
+      </c>
+      <c r="B1153" t="s">
+        <v>2334</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1154" t="s">
+        <v>2333</v>
+      </c>
+      <c r="B1154" t="s">
+        <v>2335</v>
       </c>
     </row>
   </sheetData>
@@ -16946,16 +17570,16 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2327</v>
+        <v>2325</v>
       </c>
       <c r="B2" t="s">
+        <v>2324</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2325</v>
+      </c>
+      <c r="E2" t="s">
         <v>2326</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2327</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2328</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -16991,7 +17615,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>2329</v>
+        <v>2327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modulo de registro avanzado hasta proxima visita
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7613C9-AFDD-43C9-8ED3-C0799282B5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267CE33C-6438-40F4-806A-878CE3544F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-4020" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
@@ -7530,10 +7530,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>310</v>
+        <v>220</v>
       </c>
       <c r="C2" s="3">
-        <v>45134</v>
+        <v>45135</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -7543,11 +7543,11 @@
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2" si="0">CONCATENATE(TEXT(B2,"0000"),"/",TEXT(H2,"00"))</f>
-        <v>0310/01</v>
+        <v>0220/01</v>
       </c>
       <c r="G2" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F2),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>11e39041-f9fd-45b6-94b8-c301b9910979</v>
+        <v>e2323cc1-4e59-4fb6-b892-e52d886244c9</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>2291</v>
@@ -7573,7 +7573,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>31</v>
+        <v>297</v>
       </c>
       <c r="C3" s="3">
         <v>45135</v>
@@ -7586,11 +7586,11 @@
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F8" si="1">CONCATENATE(TEXT(B3,"0000"),"/",TEXT(H3,"00"))</f>
-        <v>0031/01</v>
+        <v>0297/01</v>
       </c>
       <c r="G3" t="str">
         <f>VLOOKUP(CONCATENATE("PU/GRE/CG/",F3),Sheet1!$A$1:$B$1251,2,FALSE)</f>
-        <v>899f6639-2fee-49e4-adbd-9ac1c7d4478f</v>
+        <v>982fa04a-e022-440f-b4c3-54241e10a25d</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>2291</v>

</xml_diff>

<commit_message>
started changing database saving methods
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7655C13C-F1B5-4CEE-B04F-2355B33C85EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFF4A03-86D0-43AF-BE85-D01D432C5F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-4020" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
@@ -40,18 +40,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
-    <t>Hogar</t>
-  </si>
-  <si>
-    <t>FechaVisita</t>
-  </si>
-  <si>
-    <t>MotivoVisita</t>
-  </si>
-  <si>
-    <t>EntregaEn</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -70,24 +58,9 @@
     <t>En el SAI</t>
   </si>
   <si>
-    <t>S_GENERAL</t>
-  </si>
-  <si>
-    <t>D_GENERAL</t>
-  </si>
-  <si>
-    <t>B_SERVIDO</t>
-  </si>
-  <si>
-    <t>D_BENSERV</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
-    <t>SERVBEN</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
@@ -113,6 +86,33 @@
   </si>
   <si>
     <t>1.8</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>place</t>
+  </si>
+  <si>
+    <t>general_service</t>
+  </si>
+  <si>
+    <t>general_donor</t>
+  </si>
+  <si>
+    <t>beneficiaries_served</t>
+  </si>
+  <si>
+    <t>individual_service</t>
+  </si>
+  <si>
+    <t>individual_donor</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,46 +518,47 @@
     <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.42578125" style="1"/>
+    <col min="11" max="11" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -581,22 +582,22 @@
         <v>0270/01</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -620,22 +621,22 @@
         <v>0060/02</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -659,22 +660,22 @@
         <v>0030/02</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -708,16 +709,16 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -725,13 +726,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,13 +740,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -753,7 +754,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed some lines lenght
</commit_message>
<xml_diff>
--- a/Archivos/Servir.xlsx
+++ b/Archivos/Servir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenie\Documents\Jeniel\Programación\Phyton\Shaka\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFF4A03-86D0-43AF-BE85-D01D432C5F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BBDE3E-654E-4125-A739-B9A5518C1C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-4020" windowWidth="20730" windowHeight="11040" xr2:uid="{CC2F5BC1-99A5-4FE5-A5FB-951474DCC15C}"/>
   </bookViews>
@@ -503,8 +503,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,9 +515,9 @@
     <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>

</xml_diff>